<commit_message>
Added some test results.
</commit_message>
<xml_diff>
--- a/Coursework Part 2/results.xlsx
+++ b/Coursework Part 2/results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="46">
   <si>
     <t>Image Dimensions</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>No. of Bodies</t>
+  </si>
+  <si>
+    <t>Simulation Iterations = 1000, Blocks = 16, Threads = 128</t>
+  </si>
+  <si>
+    <t>Simulation Iterations = 1000, No. of Bodies = 512</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1519,7 @@
                   <c:v>2739.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3572.1</c:v>
+                  <c:v>2805.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7572,7 +7578,7 @@
   <dimension ref="A1:Z103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K23"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7593,7 +7599,7 @@
       </c>
       <c r="B1" s="38"/>
       <c r="G1" s="38" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H1" s="38"/>
       <c r="I1" s="38"/>
@@ -7603,7 +7609,7 @@
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
       <c r="R1" s="38" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="S1" s="38"/>
       <c r="T1" s="38"/>
@@ -7626,28 +7632,28 @@
         <v>43</v>
       </c>
       <c r="G2" s="2">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2">
-        <v>200</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2">
-        <v>300</v>
+        <v>64</v>
       </c>
       <c r="J2" s="2">
-        <v>400</v>
+        <v>128</v>
       </c>
       <c r="K2" s="2">
-        <v>500</v>
+        <v>256</v>
       </c>
       <c r="L2" s="2">
-        <v>600</v>
+        <v>512</v>
       </c>
       <c r="M2" s="2">
-        <v>700</v>
+        <v>1024</v>
       </c>
       <c r="N2" s="2">
-        <v>800</v>
+        <v>2048</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>0</v>
@@ -7754,8 +7760,8 @@
       <c r="M4" s="1">
         <v>2796</v>
       </c>
-      <c r="N4" s="1">
-        <v>3616</v>
+      <c r="N4">
+        <v>2840</v>
       </c>
       <c r="Q4" s="5">
         <v>1</v>
@@ -7818,8 +7824,8 @@
       <c r="M5" s="1">
         <v>2737</v>
       </c>
-      <c r="N5" s="1">
-        <v>3566</v>
+      <c r="N5">
+        <v>2802</v>
       </c>
       <c r="Q5" s="6">
         <v>2</v>
@@ -7870,8 +7876,8 @@
       <c r="M6" s="1">
         <v>2736</v>
       </c>
-      <c r="N6" s="1">
-        <v>3555</v>
+      <c r="N6">
+        <v>2800</v>
       </c>
       <c r="Q6" s="6">
         <v>3</v>
@@ -7922,8 +7928,8 @@
       <c r="M7" s="1">
         <v>2732</v>
       </c>
-      <c r="N7" s="1">
-        <v>3566</v>
+      <c r="N7">
+        <v>2808</v>
       </c>
       <c r="Q7" s="6">
         <v>4</v>
@@ -7974,8 +7980,8 @@
       <c r="M8" s="1">
         <v>2731</v>
       </c>
-      <c r="N8" s="1">
-        <v>3568</v>
+      <c r="N8">
+        <v>2802</v>
       </c>
       <c r="Q8" s="6">
         <v>5</v>
@@ -8026,8 +8032,8 @@
       <c r="M9" s="1">
         <v>2727</v>
       </c>
-      <c r="N9" s="1">
-        <v>3578</v>
+      <c r="N9">
+        <v>2800</v>
       </c>
       <c r="Q9" s="6">
         <v>6</v>
@@ -8051,7 +8057,7 @@
       </c>
       <c r="B10" s="10">
         <f>AVERAGE(N4:N103)</f>
-        <v>3572.1</v>
+        <v>2805.1</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="6">
@@ -8078,8 +8084,8 @@
       <c r="M10" s="1">
         <v>2743</v>
       </c>
-      <c r="N10" s="1">
-        <v>3583</v>
+      <c r="N10">
+        <v>2799</v>
       </c>
       <c r="Q10" s="6">
         <v>7</v>
@@ -8124,8 +8130,8 @@
       <c r="M11" s="1">
         <v>2723</v>
       </c>
-      <c r="N11" s="1">
-        <v>3567</v>
+      <c r="N11">
+        <v>2802</v>
       </c>
       <c r="Q11" s="6">
         <v>8</v>
@@ -8169,8 +8175,8 @@
       <c r="M12" s="1">
         <v>2742</v>
       </c>
-      <c r="N12" s="1">
-        <v>3564</v>
+      <c r="N12">
+        <v>2804</v>
       </c>
       <c r="Q12" s="6">
         <v>9</v>
@@ -8218,8 +8224,8 @@
       <c r="M13" s="1">
         <v>2726</v>
       </c>
-      <c r="N13" s="1">
-        <v>3558</v>
+      <c r="N13">
+        <v>2804</v>
       </c>
       <c r="Q13" s="6">
         <v>10</v>
@@ -8257,7 +8263,9 @@
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="N14">
+        <v>2805</v>
+      </c>
       <c r="Q14" s="6">
         <v>11</v>
       </c>
@@ -8295,7 +8303,9 @@
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="N15">
+        <v>2802</v>
+      </c>
       <c r="Q15" s="6">
         <v>12</v>
       </c>
@@ -8333,7 +8343,9 @@
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="N16">
+        <v>2806</v>
+      </c>
       <c r="Q16" s="6">
         <v>13</v>
       </c>
@@ -8371,7 +8383,9 @@
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="N17">
+        <v>2803</v>
+      </c>
       <c r="Q17" s="6">
         <v>14</v>
       </c>
@@ -8409,7 +8423,9 @@
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="N18">
+        <v>2805</v>
+      </c>
       <c r="Q18" s="6">
         <v>15</v>
       </c>
@@ -8440,7 +8456,9 @@
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+      <c r="N19">
+        <v>2804</v>
+      </c>
       <c r="Q19" s="6">
         <v>16</v>
       </c>
@@ -8477,7 +8495,9 @@
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="N20">
+        <v>2805</v>
+      </c>
       <c r="Q20" s="6">
         <v>17</v>
       </c>
@@ -8508,7 +8528,9 @@
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="N21">
+        <v>2803</v>
+      </c>
       <c r="Q21" s="6">
         <v>18</v>
       </c>
@@ -8544,7 +8566,9 @@
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="N22">
+        <v>2802</v>
+      </c>
       <c r="Q22" s="6">
         <v>19</v>
       </c>
@@ -8584,7 +8608,9 @@
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="N23">
+        <v>2806</v>
+      </c>
       <c r="Q23" s="6">
         <v>20</v>
       </c>
@@ -8873,11 +8899,11 @@
       </c>
       <c r="B31" s="30">
         <f>'Seq. Results'!B10/OMP!B10</f>
-        <v>1</v>
+        <v>1.2734305372357493</v>
       </c>
       <c r="C31" s="32">
         <f>B31/B20</f>
-        <v>0.25</v>
+        <v>0.31835763430893732</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="6"/>

</xml_diff>

<commit_message>
Done initial analysis and introduction.
</commit_message>
<xml_diff>
--- a/Coursework Part 2/results.xlsx
+++ b/Coursework Part 2/results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beej\Documents\Work\C&amp;PS\Coursework\Concurrent-And-Parallel-Systems-CW\Coursework Part 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beej\Documents\Work\C&amp;PS\Concurrent-And-Parallel-Systems-CW\Coursework Part 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Seq Graph" sheetId="14" r:id="rId1"/>
@@ -844,15 +844,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -863,6 +854,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1131,7 +1131,9 @@
       <c:valAx>
         <c:axId val="539109520"/>
         <c:scaling>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
+          <c:min val="16"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6368,7 +6370,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="95" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6424,7 +6426,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659091" cy="6280727"/>
+    <xdr:ext cx="8654716" cy="6272463"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6952,7 +6954,7 @@
   <dimension ref="A1:W103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6977,32 +6979,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="37"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
       <c r="N1" s="17"/>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
       <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -7079,27 +7081,27 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
       <c r="N3" s="17"/>
       <c r="P3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="Q3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
       <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -7507,10 +7509,10 @@
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="33"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -7559,10 +7561,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="37"/>
       <c r="D12" s="4" t="s">
         <v>34</v>
       </c>
@@ -7626,7 +7628,7 @@
       <c r="D13" s="6">
         <v>64</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="33">
         <f>_xlfn.STDEV.S(G4:G103)</f>
         <v>0.88642967896927705</v>
       </c>
@@ -7688,7 +7690,7 @@
       <c r="D14" s="6">
         <v>128</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="33">
         <f>_xlfn.STDEV.P(H4:H103)</f>
         <v>1.9165333286953303</v>
       </c>
@@ -7751,7 +7753,7 @@
       <c r="D15" s="6">
         <v>256</v>
       </c>
-      <c r="E15" s="36">
+      <c r="E15" s="33">
         <f>_xlfn.STDEV.P(I4:I103)</f>
         <v>3.6821732713168225</v>
       </c>
@@ -7814,7 +7816,7 @@
       <c r="D16" s="6">
         <v>512</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="33">
         <f>_xlfn.STDEV.P(J4:J103)</f>
         <v>8.0935221010385856</v>
       </c>
@@ -7877,7 +7879,7 @@
       <c r="D17" s="6">
         <v>1024</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="33">
         <f>_xlfn.STDEV.P(K4:K103)</f>
         <v>17.878129096748353</v>
       </c>
@@ -7940,7 +7942,7 @@
       <c r="D18" s="6">
         <v>2048</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="33">
         <f>_xlfn.STDEV.P(L4:L103)</f>
         <v>26.909438864457961</v>
       </c>
@@ -8003,7 +8005,7 @@
       <c r="D19" s="6">
         <v>4096</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="33">
         <f>_xlfn.STDEV.P(M4:M103)</f>
         <v>106.66347828568124</v>
       </c>
@@ -10427,23 +10429,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="37"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
       <c r="S1" s="21"/>
@@ -10511,15 +10513,15 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
       <c r="O3" s="10"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="21"/>
@@ -10843,10 +10845,10 @@
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="33"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -10930,7 +10932,7 @@
       <c r="D13" s="6">
         <v>64</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="33">
         <f>_xlfn.STDEV.S(G4:G103)</f>
         <v>4.9347663766301233</v>
       </c>
@@ -10975,7 +10977,7 @@
       <c r="D14" s="6">
         <v>128</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="33">
         <f>_xlfn.STDEV.P(H4:H103)</f>
         <v>2.8484908284914683</v>
       </c>
@@ -11020,7 +11022,7 @@
       <c r="D15" s="6">
         <v>256</v>
       </c>
-      <c r="E15" s="36">
+      <c r="E15" s="33">
         <f>_xlfn.STDEV.P(I4:I103)</f>
         <v>4.0204974816557204</v>
       </c>
@@ -11065,7 +11067,7 @@
       <c r="D16" s="6">
         <v>512</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="33">
         <f>_xlfn.STDEV.P(J4:J103)</f>
         <v>6.6033627796752139</v>
       </c>
@@ -11110,7 +11112,7 @@
       <c r="D17" s="6">
         <v>1024</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="33">
         <f>_xlfn.STDEV.P(K4:K103)</f>
         <v>14.427539637789939</v>
       </c>
@@ -11155,7 +11157,7 @@
       <c r="D18" s="6">
         <v>2048</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="33">
         <f>_xlfn.STDEV.P(L4:L103)</f>
         <v>34.954969603763068</v>
       </c>
@@ -11200,7 +11202,7 @@
       <c r="D19" s="6">
         <v>4096</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="33">
         <f>_xlfn.STDEV.P(M4:M103)</f>
         <v>82.886232270504365</v>
       </c>
@@ -13606,32 +13608,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="37"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
       <c r="N1" s="17"/>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
       <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -13708,27 +13710,27 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
       <c r="N3" s="17"/>
       <c r="P3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="Q3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
       <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -14136,10 +14138,10 @@
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="33"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -14188,10 +14190,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="37"/>
       <c r="D12" s="4" t="s">
         <v>34</v>
       </c>
@@ -14255,7 +14257,7 @@
       <c r="D13" s="6">
         <v>64</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="33">
         <f>_xlfn.STDEV.S(G4:G103)</f>
         <v>4.5579877715119563</v>
       </c>
@@ -14317,7 +14319,7 @@
       <c r="D14" s="6">
         <v>128</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="33">
         <f>_xlfn.STDEV.P(H4:H103)</f>
         <v>4.889366012071501</v>
       </c>
@@ -14380,7 +14382,7 @@
       <c r="D15" s="6">
         <v>256</v>
       </c>
-      <c r="E15" s="36">
+      <c r="E15" s="33">
         <f>_xlfn.STDEV.P(I4:I103)</f>
         <v>4.1820569101818679</v>
       </c>
@@ -14443,7 +14445,7 @@
       <c r="D16" s="6">
         <v>512</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="33">
         <f>_xlfn.STDEV.P(J4:J103)</f>
         <v>4.9844157129998719</v>
       </c>
@@ -14506,7 +14508,7 @@
       <c r="D17" s="6">
         <v>1024</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="33">
         <f>_xlfn.STDEV.P(K4:K103)</f>
         <v>4.7634441321380052</v>
       </c>
@@ -14569,7 +14571,7 @@
       <c r="D18" s="6">
         <v>2048</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="33">
         <f>_xlfn.STDEV.P(L4:L103)</f>
         <v>12.65115014534252</v>
       </c>
@@ -14632,7 +14634,7 @@
       <c r="D19" s="6">
         <v>4096</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="33">
         <f>_xlfn.STDEV.P(M4:M103)</f>
         <v>26.363884387548069</v>
       </c>
@@ -14843,11 +14845,11 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
       <c r="D23"/>
       <c r="E23" s="1"/>
       <c r="F23" s="6">
@@ -14960,11 +14962,11 @@
       <c r="A25" s="6">
         <v>4</v>
       </c>
-      <c r="B25" s="37">
+      <c r="B25" s="34">
         <f>'[1]Seq. Results'!B4/'[1]Manual Threading'!B4</f>
         <v>4.6029182646212847</v>
       </c>
-      <c r="C25" s="38" t="e">
+      <c r="C25" s="35" t="e">
         <f>B25/B21</f>
         <v>#DIV/0!</v>
       </c>
@@ -15021,11 +15023,11 @@
       <c r="A26" s="6">
         <v>8</v>
       </c>
-      <c r="B26" s="37">
+      <c r="B26" s="34">
         <f>'[1]Seq. Results'!B5/'[1]Manual Threading'!B5</f>
         <v>4.7106701356281846</v>
       </c>
-      <c r="C26" s="39" t="e">
+      <c r="C26" s="36" t="e">
         <f>B26/B21</f>
         <v>#DIV/0!</v>
       </c>
@@ -15081,11 +15083,11 @@
       <c r="A27" s="6">
         <v>16</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B27" s="34">
         <f>'[1]Seq. Results'!B6/'[1]Manual Threading'!B6</f>
         <v>4.8492850742198153</v>
       </c>
-      <c r="C27" s="39" t="e">
+      <c r="C27" s="36" t="e">
         <f>B27/B21</f>
         <v>#DIV/0!</v>
       </c>
@@ -15141,11 +15143,11 @@
       <c r="A28" s="6">
         <v>32</v>
       </c>
-      <c r="B28" s="37">
+      <c r="B28" s="34">
         <f>'[1]Seq. Results'!B7/'[1]Manual Threading'!B7</f>
         <v>4.8671166527261764</v>
       </c>
-      <c r="C28" s="39" t="e">
+      <c r="C28" s="36" t="e">
         <f>B28/B21</f>
         <v>#DIV/0!</v>
       </c>
@@ -15201,11 +15203,11 @@
       <c r="A29" s="6">
         <v>64</v>
       </c>
-      <c r="B29" s="37">
+      <c r="B29" s="34">
         <f>'[1]Seq. Results'!B8/'[1]Manual Threading'!B8</f>
         <v>4.8120552081086911</v>
       </c>
-      <c r="C29" s="39" t="e">
+      <c r="C29" s="36" t="e">
         <f>B29/B21</f>
         <v>#DIV/0!</v>
       </c>
@@ -15261,11 +15263,11 @@
       <c r="A30" s="6">
         <v>128</v>
       </c>
-      <c r="B30" s="37">
+      <c r="B30" s="34">
         <f>'[1]Seq. Results'!B9/'[1]Manual Threading'!B9</f>
         <v>4.7611160133111214</v>
       </c>
-      <c r="C30" s="39" t="e">
+      <c r="C30" s="36" t="e">
         <f>B30/B21</f>
         <v>#DIV/0!</v>
       </c>
@@ -15321,11 +15323,11 @@
       <c r="A31" s="6">
         <v>256</v>
       </c>
-      <c r="B31" s="37">
+      <c r="B31" s="34">
         <f>'[1]Seq. Results'!B10/'[1]Manual Threading'!B10</f>
         <v>4.6812327506899729</v>
       </c>
-      <c r="C31" s="39" t="e">
+      <c r="C31" s="36" t="e">
         <f>B31/B21</f>
         <v>#DIV/0!</v>
       </c>
@@ -15381,11 +15383,11 @@
       <c r="A32" s="6">
         <v>512</v>
       </c>
-      <c r="B32" s="37" t="e">
+      <c r="B32" s="34" t="e">
         <f>'[1]Seq. Results'!B11/'[1]Manual Threading'!B11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C32" s="39" t="e">
+      <c r="C32" s="36" t="e">
         <f>B32/B21</f>
         <v>#DIV/0!</v>
       </c>
@@ -18788,14 +18790,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="Q3:V3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G1:M1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="Q3:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18821,12 +18823,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
@@ -19672,11 +19674,11 @@
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="17"/>
       <c r="K10" s="1">
         <v>6</v>
@@ -19927,10 +19929,10 @@
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="35"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="17"/>
       <c r="K12" s="1">
         <v>8</v>

</xml_diff>

<commit_message>
Working on results, trip to tesco safety commit.
</commit_message>
<xml_diff>
--- a/Coursework Part 2/results.xlsx
+++ b/Coursework Part 2/results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40183743\Documents\Concurrent-And-Parallel-Systems-CW\Coursework Part 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beej\Documents\Work\C&amp;PS\Concurrent-And-Parallel-Systems-CW\Coursework Part 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Seq. Results" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Comparison 4" sheetId="15" r:id="rId8"/>
     <sheet name="Seq Graph" sheetId="14" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -823,15 +823,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -842,8 +833,23 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -851,14 +857,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -958,7 +958,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1070,7 +1069,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1273,7 +1271,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1394,7 +1391,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1534,7 +1530,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1636,7 +1631,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1862,7 +1856,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2002,7 +1995,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2544,7 +2536,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2666,7 +2657,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2747,7 +2737,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2844,7 +2833,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3256,7 +3244,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3377,7 +3364,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3458,7 +3444,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3530,7 +3515,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3593,10 +3577,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Seq. Results'!$A$3:$A$10</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Seq. Results'!$A$3:$A$10</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Seq. Results'!$A$3:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>64</c:v>
                 </c:pt>
@@ -3623,10 +3614,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Seq. Results'!$B$3:$B$10</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Seq. Results'!$B$3:$B$9</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Seq. Results'!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>20.39</c:v>
                 </c:pt>
@@ -6564,7 +6562,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6610,7 +6608,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="99" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6621,13 +6619,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660876" cy="6294356"/>
+    <xdr:ext cx="8656948" cy="6276680"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6654,7 +6652,73 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660876" cy="6294356"/>
+    <xdr:ext cx="8656948" cy="6276680"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656948" cy="6276680"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656948" cy="6276680"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6683,77 +6747,17 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660876" cy="6294356"/>
+    <xdr:ext cx="8659091" cy="6280727"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660876" cy="6294356"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669364" cy="6288114"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7042,60 +7046,60 @@
   <dimension ref="A1:W103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B3" sqref="B3:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="19"/>
-    <col min="4" max="4" width="12.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="19"/>
-    <col min="9" max="9" width="9.140625" style="19" customWidth="1"/>
-    <col min="10" max="15" width="9.140625" style="19"/>
-    <col min="16" max="16" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="19" customWidth="1"/>
-    <col min="18" max="22" width="9.140625" style="19"/>
-    <col min="23" max="23" width="9.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="17.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="19"/>
+    <col min="4" max="4" width="12.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" style="19"/>
+    <col min="9" max="9" width="9.109375" style="19" customWidth="1"/>
+    <col min="10" max="15" width="9.109375" style="19"/>
+    <col min="16" max="16" width="9.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="19" customWidth="1"/>
+    <col min="18" max="22" width="9.109375" style="19"/>
+    <col min="23" max="23" width="9.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="43"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
       <c r="N1" s="17"/>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
       <c r="W1" s="17"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -7155,7 +7159,7 @@
       </c>
       <c r="W2" s="23"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>64</v>
       </c>
@@ -7169,30 +7173,30 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
       <c r="N3" s="17"/>
       <c r="P3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="Q3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="45"/>
       <c r="W3" s="17"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>128</v>
       </c>
@@ -7250,7 +7254,7 @@
         <v>7846</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>256</v>
       </c>
@@ -7308,7 +7312,7 @@
         <v>7793</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>512</v>
       </c>
@@ -7366,7 +7370,7 @@
         <v>7791</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1024</v>
       </c>
@@ -7424,7 +7428,7 @@
         <v>7827</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2048</v>
       </c>
@@ -7482,7 +7486,7 @@
         <v>7829</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>4096</v>
       </c>
@@ -7540,7 +7544,7 @@
         <v>7819</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="7"/>
       <c r="C10"/>
@@ -7593,14 +7597,14 @@
         <v>7814</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -7648,11 +7652,11 @@
         <v>7805</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="37"/>
+      <c r="B12" s="43"/>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
@@ -7706,7 +7710,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>10</v>
       </c>
@@ -7767,7 +7771,7 @@
         <v>7781</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
         <v>250</v>
       </c>
@@ -7829,7 +7833,7 @@
         <v>7778</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>500</v>
       </c>
@@ -7892,7 +7896,7 @@
         <v>7799</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>750</v>
       </c>
@@ -7955,7 +7959,7 @@
         <v>7771</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>1000</v>
       </c>
@@ -8018,7 +8022,7 @@
         <v>7794</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>1250</v>
       </c>
@@ -8081,7 +8085,7 @@
         <v>7791</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>1500</v>
       </c>
@@ -8144,7 +8148,7 @@
         <v>7804</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="7"/>
       <c r="C20"/>
@@ -8197,7 +8201,7 @@
         <v>7778</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -8250,7 +8254,7 @@
         <v>7785</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -8303,7 +8307,7 @@
         <v>7797</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -8356,7 +8360,7 @@
         <v>7789</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -8388,7 +8392,7 @@
       </c>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -8420,7 +8424,7 @@
       </c>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E26" s="1"/>
       <c r="F26" s="6">
         <v>23</v>
@@ -8448,7 +8452,7 @@
       </c>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E27" s="1"/>
       <c r="F27" s="6">
         <v>24</v>
@@ -8476,7 +8480,7 @@
       </c>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E28" s="1"/>
       <c r="F28" s="6">
         <v>25</v>
@@ -8504,7 +8508,7 @@
       </c>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E29" s="1"/>
       <c r="F29" s="6">
         <v>26</v>
@@ -8532,7 +8536,7 @@
       </c>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
       <c r="F30" s="6">
         <v>27</v>
@@ -8560,7 +8564,7 @@
       </c>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
       <c r="F31" s="6">
         <v>28</v>
@@ -8588,7 +8592,7 @@
       </c>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E32" s="1"/>
       <c r="F32" s="6">
         <v>29</v>
@@ -8616,7 +8620,7 @@
       </c>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E33" s="1"/>
       <c r="F33" s="6">
         <v>30</v>
@@ -8644,7 +8648,7 @@
       </c>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
       <c r="F34" s="6">
         <v>31</v>
@@ -8672,7 +8676,7 @@
       </c>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
       <c r="F35" s="6">
         <v>32</v>
@@ -8700,7 +8704,7 @@
       </c>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
       <c r="F36" s="6">
         <v>33</v>
@@ -8728,7 +8732,7 @@
       </c>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E37" s="1"/>
       <c r="F37" s="6">
         <v>34</v>
@@ -8756,7 +8760,7 @@
       </c>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
       <c r="F38" s="6">
         <v>35</v>
@@ -8784,7 +8788,7 @@
       </c>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F39" s="6">
         <v>36</v>
       </c>
@@ -8810,7 +8814,7 @@
         <v>80691</v>
       </c>
     </row>
-    <row r="40" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F40" s="6">
         <v>37</v>
       </c>
@@ -8836,7 +8840,7 @@
         <v>80861</v>
       </c>
     </row>
-    <row r="41" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F41" s="6">
         <v>38</v>
       </c>
@@ -8862,7 +8866,7 @@
         <v>80766</v>
       </c>
     </row>
-    <row r="42" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F42" s="6">
         <v>39</v>
       </c>
@@ -8888,7 +8892,7 @@
         <v>80886</v>
       </c>
     </row>
-    <row r="43" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F43" s="6">
         <v>40</v>
       </c>
@@ -8914,7 +8918,7 @@
         <v>80879</v>
       </c>
     </row>
-    <row r="44" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F44" s="6">
         <v>41</v>
       </c>
@@ -8940,7 +8944,7 @@
         <v>80627</v>
       </c>
     </row>
-    <row r="45" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F45" s="6">
         <v>42</v>
       </c>
@@ -8966,7 +8970,7 @@
         <v>81188</v>
       </c>
     </row>
-    <row r="46" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F46" s="6">
         <v>43</v>
       </c>
@@ -8992,7 +8996,7 @@
         <v>80892</v>
       </c>
     </row>
-    <row r="47" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F47" s="6">
         <v>44</v>
       </c>
@@ -9018,7 +9022,7 @@
         <v>80883</v>
       </c>
     </row>
-    <row r="48" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F48" s="6">
         <v>45</v>
       </c>
@@ -9044,7 +9048,7 @@
         <v>80638</v>
       </c>
     </row>
-    <row r="49" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F49" s="6">
         <v>46</v>
       </c>
@@ -9070,7 +9074,7 @@
         <v>80684</v>
       </c>
     </row>
-    <row r="50" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F50" s="6">
         <v>47</v>
       </c>
@@ -9096,7 +9100,7 @@
         <v>80887</v>
       </c>
     </row>
-    <row r="51" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F51" s="6">
         <v>48</v>
       </c>
@@ -9122,7 +9126,7 @@
         <v>80700</v>
       </c>
     </row>
-    <row r="52" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F52" s="6">
         <v>49</v>
       </c>
@@ -9148,7 +9152,7 @@
         <v>80673</v>
       </c>
     </row>
-    <row r="53" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F53" s="6">
         <v>50</v>
       </c>
@@ -9174,7 +9178,7 @@
         <v>80685</v>
       </c>
     </row>
-    <row r="54" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F54" s="6">
         <v>51</v>
       </c>
@@ -9200,7 +9204,7 @@
         <v>80767</v>
       </c>
     </row>
-    <row r="55" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F55" s="6">
         <v>52</v>
       </c>
@@ -9226,7 +9230,7 @@
         <v>80639</v>
       </c>
     </row>
-    <row r="56" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F56" s="6">
         <v>53</v>
       </c>
@@ -9252,7 +9256,7 @@
         <v>80766</v>
       </c>
     </row>
-    <row r="57" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F57" s="6">
         <v>54</v>
       </c>
@@ -9278,7 +9282,7 @@
         <v>80810</v>
       </c>
     </row>
-    <row r="58" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F58" s="6">
         <v>55</v>
       </c>
@@ -9304,7 +9308,7 @@
         <v>80936</v>
       </c>
     </row>
-    <row r="59" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F59" s="6">
         <v>56</v>
       </c>
@@ -9330,7 +9334,7 @@
         <v>80938</v>
       </c>
     </row>
-    <row r="60" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F60" s="6">
         <v>57</v>
       </c>
@@ -9356,7 +9360,7 @@
         <v>80897</v>
       </c>
     </row>
-    <row r="61" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F61" s="6">
         <v>58</v>
       </c>
@@ -9382,7 +9386,7 @@
         <v>80807</v>
       </c>
     </row>
-    <row r="62" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F62" s="6">
         <v>59</v>
       </c>
@@ -9408,7 +9412,7 @@
         <v>80627</v>
       </c>
     </row>
-    <row r="63" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F63" s="6">
         <v>60</v>
       </c>
@@ -9434,7 +9438,7 @@
         <v>80703</v>
       </c>
     </row>
-    <row r="64" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F64" s="6">
         <v>61</v>
       </c>
@@ -9460,7 +9464,7 @@
         <v>80712</v>
       </c>
     </row>
-    <row r="65" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F65" s="6">
         <v>62</v>
       </c>
@@ -9486,7 +9490,7 @@
         <v>80753</v>
       </c>
     </row>
-    <row r="66" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F66" s="6">
         <v>63</v>
       </c>
@@ -9512,7 +9516,7 @@
         <v>80774</v>
       </c>
     </row>
-    <row r="67" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F67" s="6">
         <v>64</v>
       </c>
@@ -9538,7 +9542,7 @@
         <v>80865</v>
       </c>
     </row>
-    <row r="68" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F68" s="6">
         <v>65</v>
       </c>
@@ -9564,7 +9568,7 @@
         <v>80912</v>
       </c>
     </row>
-    <row r="69" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F69" s="6">
         <v>66</v>
       </c>
@@ -9590,7 +9594,7 @@
         <v>80725</v>
       </c>
     </row>
-    <row r="70" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F70" s="6">
         <v>67</v>
       </c>
@@ -9616,7 +9620,7 @@
         <v>80774</v>
       </c>
     </row>
-    <row r="71" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F71" s="6">
         <v>68</v>
       </c>
@@ -9642,7 +9646,7 @@
         <v>80681</v>
       </c>
     </row>
-    <row r="72" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F72" s="6">
         <v>69</v>
       </c>
@@ -9668,7 +9672,7 @@
         <v>80746</v>
       </c>
     </row>
-    <row r="73" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F73" s="6">
         <v>70</v>
       </c>
@@ -9694,7 +9698,7 @@
         <v>80660</v>
       </c>
     </row>
-    <row r="74" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F74" s="6">
         <v>71</v>
       </c>
@@ -9720,7 +9724,7 @@
         <v>80950</v>
       </c>
     </row>
-    <row r="75" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F75" s="6">
         <v>72</v>
       </c>
@@ -9746,7 +9750,7 @@
         <v>80844</v>
       </c>
     </row>
-    <row r="76" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F76" s="6">
         <v>73</v>
       </c>
@@ -9772,7 +9776,7 @@
         <v>80902</v>
       </c>
     </row>
-    <row r="77" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F77" s="6">
         <v>74</v>
       </c>
@@ -9798,7 +9802,7 @@
         <v>80838</v>
       </c>
     </row>
-    <row r="78" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F78" s="6">
         <v>75</v>
       </c>
@@ -9824,7 +9828,7 @@
         <v>80765</v>
       </c>
     </row>
-    <row r="79" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F79" s="6">
         <v>76</v>
       </c>
@@ -9850,7 +9854,7 @@
         <v>80945</v>
       </c>
     </row>
-    <row r="80" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F80" s="6">
         <v>77</v>
       </c>
@@ -9876,7 +9880,7 @@
         <v>80835</v>
       </c>
     </row>
-    <row r="81" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F81" s="6">
         <v>78</v>
       </c>
@@ -9902,7 +9906,7 @@
         <v>80863</v>
       </c>
     </row>
-    <row r="82" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F82" s="6">
         <v>79</v>
       </c>
@@ -9928,7 +9932,7 @@
         <v>80798</v>
       </c>
     </row>
-    <row r="83" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F83" s="6">
         <v>80</v>
       </c>
@@ -9954,7 +9958,7 @@
         <v>80767</v>
       </c>
     </row>
-    <row r="84" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F84" s="6">
         <v>81</v>
       </c>
@@ -9980,7 +9984,7 @@
         <v>80641</v>
       </c>
     </row>
-    <row r="85" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F85" s="6">
         <v>82</v>
       </c>
@@ -10006,7 +10010,7 @@
         <v>80648</v>
       </c>
     </row>
-    <row r="86" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F86" s="6">
         <v>83</v>
       </c>
@@ -10032,7 +10036,7 @@
         <v>80833</v>
       </c>
     </row>
-    <row r="87" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F87" s="6">
         <v>84</v>
       </c>
@@ -10058,7 +10062,7 @@
         <v>80847</v>
       </c>
     </row>
-    <row r="88" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F88" s="6">
         <v>85</v>
       </c>
@@ -10084,7 +10088,7 @@
         <v>80763</v>
       </c>
     </row>
-    <row r="89" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F89" s="6">
         <v>86</v>
       </c>
@@ -10110,7 +10114,7 @@
         <v>80690</v>
       </c>
     </row>
-    <row r="90" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F90" s="6">
         <v>87</v>
       </c>
@@ -10136,7 +10140,7 @@
         <v>80652</v>
       </c>
     </row>
-    <row r="91" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F91" s="6">
         <v>88</v>
       </c>
@@ -10162,7 +10166,7 @@
         <v>80782</v>
       </c>
     </row>
-    <row r="92" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F92" s="6">
         <v>89</v>
       </c>
@@ -10188,7 +10192,7 @@
         <v>80832</v>
       </c>
     </row>
-    <row r="93" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F93" s="6">
         <v>90</v>
       </c>
@@ -10214,7 +10218,7 @@
         <v>80753</v>
       </c>
     </row>
-    <row r="94" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F94" s="6">
         <v>91</v>
       </c>
@@ -10240,7 +10244,7 @@
         <v>80909</v>
       </c>
     </row>
-    <row r="95" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F95" s="6">
         <v>92</v>
       </c>
@@ -10266,7 +10270,7 @@
         <v>80917</v>
       </c>
     </row>
-    <row r="96" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F96" s="6">
         <v>93</v>
       </c>
@@ -10292,7 +10296,7 @@
         <v>80884</v>
       </c>
     </row>
-    <row r="97" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F97" s="6">
         <v>94</v>
       </c>
@@ -10318,7 +10322,7 @@
         <v>80922</v>
       </c>
     </row>
-    <row r="98" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F98" s="6">
         <v>95</v>
       </c>
@@ -10344,7 +10348,7 @@
         <v>80738</v>
       </c>
     </row>
-    <row r="99" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F99" s="6">
         <v>96</v>
       </c>
@@ -10370,7 +10374,7 @@
         <v>80671</v>
       </c>
     </row>
-    <row r="100" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F100" s="6">
         <v>97</v>
       </c>
@@ -10396,7 +10400,7 @@
         <v>80870</v>
       </c>
     </row>
-    <row r="101" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F101" s="6">
         <v>98</v>
       </c>
@@ -10422,7 +10426,7 @@
         <v>80742</v>
       </c>
     </row>
-    <row r="102" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F102" s="6">
         <v>99</v>
       </c>
@@ -10448,7 +10452,7 @@
         <v>80627</v>
       </c>
     </row>
-    <row r="103" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F103" s="6">
         <v>100</v>
       </c>
@@ -10493,47 +10497,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V104"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="9.140625" style="17"/>
-    <col min="15" max="15" width="12.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="17" customWidth="1"/>
-    <col min="18" max="23" width="9.140625" style="17"/>
-    <col min="24" max="24" width="17.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="17.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="9.109375" style="17"/>
+    <col min="15" max="15" width="12.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="17" customWidth="1"/>
+    <col min="18" max="23" width="9.109375" style="17"/>
+    <col min="24" max="24" width="17.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="43"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
       <c r="Q1" s="19"/>
       <c r="R1" s="19"/>
       <c r="S1" s="19"/>
@@ -10541,7 +10545,7 @@
       <c r="U1" s="19"/>
       <c r="V1" s="19"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -10587,7 +10591,7 @@
       <c r="U2" s="19"/>
       <c r="V2" s="19"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>64</v>
       </c>
@@ -10601,15 +10605,15 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
       <c r="O3" s="10"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="19"/>
@@ -10619,7 +10623,7 @@
       <c r="U3" s="19"/>
       <c r="V3" s="19"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>128</v>
       </c>
@@ -10664,7 +10668,7 @@
       <c r="U4" s="19"/>
       <c r="V4" s="19"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>256</v>
       </c>
@@ -10709,7 +10713,7 @@
       <c r="U5" s="19"/>
       <c r="V5" s="19"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>512</v>
       </c>
@@ -10754,7 +10758,7 @@
       <c r="U6" s="19"/>
       <c r="V6" s="19"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1024</v>
       </c>
@@ -10799,7 +10803,7 @@
       <c r="U7" s="19"/>
       <c r="V7" s="19"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2048</v>
       </c>
@@ -10844,7 +10848,7 @@
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>4096</v>
       </c>
@@ -10889,7 +10893,7 @@
       <c r="U9" s="19"/>
       <c r="V9" s="19"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="7"/>
       <c r="C10"/>
@@ -10929,14 +10933,14 @@
       <c r="U10" s="19"/>
       <c r="V10" s="19"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -10971,7 +10975,7 @@
       <c r="U11" s="19"/>
       <c r="V11" s="19"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C12" s="19"/>
       <c r="D12" s="4" t="s">
         <v>9</v>
@@ -11013,7 +11017,7 @@
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="29"/>
       <c r="B13" s="29"/>
       <c r="C13" s="19"/>
@@ -11058,7 +11062,7 @@
       <c r="U13" s="19"/>
       <c r="V13" s="19"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -11103,7 +11107,7 @@
       <c r="U14" s="19"/>
       <c r="V14" s="19"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="18"/>
       <c r="C15"/>
@@ -11148,7 +11152,7 @@
       <c r="U15" s="19"/>
       <c r="V15" s="19"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="18"/>
       <c r="C16"/>
@@ -11193,7 +11197,7 @@
       <c r="U16" s="19"/>
       <c r="V16" s="19"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="18"/>
       <c r="C17"/>
@@ -11238,7 +11242,7 @@
       <c r="U17" s="19"/>
       <c r="V17" s="19"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="18"/>
       <c r="C18"/>
@@ -11283,7 +11287,7 @@
       <c r="U18" s="19"/>
       <c r="V18" s="19"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="18"/>
       <c r="C19"/>
@@ -11328,8 +11332,8 @@
       <c r="U19" s="19"/>
       <c r="V19" s="19"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1">
@@ -11372,7 +11376,7 @@
       <c r="U20" s="19"/>
       <c r="V20" s="19"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -11412,12 +11416,12 @@
       <c r="U21" s="19"/>
       <c r="V21" s="19"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
       <c r="D22"/>
       <c r="E22" s="1"/>
       <c r="F22" s="6">
@@ -11454,7 +11458,7 @@
       <c r="U22" s="19"/>
       <c r="V22" s="19"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -11500,7 +11504,7 @@
       <c r="U23" s="19"/>
       <c r="V23" s="19"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>64</v>
       </c>
@@ -11538,7 +11542,7 @@
         <v>30528</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>128</v>
       </c>
@@ -11576,7 +11580,7 @@
         <v>30525</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>256</v>
       </c>
@@ -11614,7 +11618,7 @@
         <v>30651</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>512</v>
       </c>
@@ -11652,7 +11656,7 @@
         <v>30606</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>1024</v>
       </c>
@@ -11690,7 +11694,7 @@
         <v>30659</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>2048</v>
       </c>
@@ -11728,7 +11732,7 @@
         <v>30664</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>4096</v>
       </c>
@@ -11766,10 +11770,10 @@
         <v>30537</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
       <c r="E31" s="29"/>
       <c r="F31" s="6">
         <v>28</v>
@@ -11796,7 +11800,7 @@
         <v>30532</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E32" s="29"/>
       <c r="F32" s="6">
         <v>29</v>
@@ -11823,11 +11827,11 @@
         <v>30532</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="37" t="s">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B33" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="37"/>
+      <c r="C33" s="43"/>
       <c r="E33" s="29"/>
       <c r="F33" s="6">
         <v>30</v>
@@ -11854,7 +11858,7 @@
         <v>30741</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
         <v>26</v>
       </c>
@@ -11887,12 +11891,12 @@
         <v>30737</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="16">
         <f>('Seq. Results'!B3+'Seq. Results'!E13)/(B3-E13) - B24</f>
         <v>0.70258118667418334</v>
       </c>
-      <c r="C35" s="49">
+      <c r="C35" s="42">
         <f>B24-('Seq. Results'!B3-'Seq. Results'!E13)/(B3+E13)</f>
         <v>0.36258474319194878</v>
       </c>
@@ -11922,12 +11926,12 @@
         <v>30589</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="16">
         <f>('Seq. Results'!B4+'Seq. Results'!E14)/(B4-E14) - B25</f>
         <v>0.16165805732390792</v>
       </c>
-      <c r="C36" s="49">
+      <c r="C36" s="42">
         <f>B25-('Seq. Results'!B4-'Seq. Results'!E14)/(B4+E14)</f>
         <v>0.14273098063910172</v>
       </c>
@@ -11957,12 +11961,12 @@
         <v>30683</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="16">
         <f>('Seq. Results'!B5+'Seq. Results'!E15)/(B5-E15) - B26</f>
         <v>8.5845150951798566E-2</v>
       </c>
-      <c r="C37" s="49">
+      <c r="C37" s="42">
         <f>B26-('Seq. Results'!B5-'Seq. Results'!E15)/(B5+E15)</f>
         <v>8.1324073028856247E-2</v>
       </c>
@@ -11992,12 +11996,12 @@
         <v>30647</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="16">
         <f>('Seq. Results'!B6+'Seq. Results'!E16)/(B6-E16) - B27</f>
         <v>4.5619616129352281E-2</v>
       </c>
-      <c r="C38" s="49">
+      <c r="C38" s="42">
         <f>B27-('Seq. Results'!B6-'Seq. Results'!E16)/(B6+E16)</f>
         <v>4.4504445655375591E-2</v>
       </c>
@@ -12027,12 +12031,12 @@
         <v>30657</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="16">
         <f>('Seq. Results'!B7+'Seq. Results'!E17)/(B7-E17) - B28</f>
         <v>2.7423242309130291E-2</v>
       </c>
-      <c r="C39" s="49">
+      <c r="C39" s="42">
         <f>B28-('Seq. Results'!B7-'Seq. Results'!E17)/(B7+E17)</f>
         <v>2.703194315890034E-2</v>
       </c>
@@ -12062,12 +12066,12 @@
         <v>30690</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="16">
         <f>('Seq. Results'!B8+'Seq. Results'!E18)/(B8-E18) - B29</f>
         <v>1.5052984168606454E-2</v>
       </c>
-      <c r="C40" s="49">
+      <c r="C40" s="42">
         <f>B29-('Seq. Results'!B8-'Seq. Results'!E18)/(B8+E18)</f>
         <v>1.4919011170357432E-2</v>
       </c>
@@ -12097,12 +12101,12 @@
         <v>30517</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="16">
         <f>('Seq. Results'!B9+'Seq. Results'!E19)/(B9-E19) - B30</f>
         <v>1.0649894364752832E-2</v>
       </c>
-      <c r="C41" s="49">
+      <c r="C41" s="42">
         <f>B30-('Seq. Results'!B9-'Seq. Results'!E19)/(B9+E19)</f>
         <v>1.0592409712171236E-2</v>
       </c>
@@ -12132,7 +12136,7 @@
         <v>30748</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E42" s="29"/>
       <c r="F42" s="6">
         <v>39</v>
@@ -12159,7 +12163,7 @@
         <v>30763</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E43" s="29"/>
       <c r="F43" s="6">
         <v>40</v>
@@ -12186,7 +12190,7 @@
         <v>30531</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E44" s="29"/>
       <c r="F44" s="6">
         <v>41</v>
@@ -12213,7 +12217,7 @@
         <v>30541</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E45" s="29"/>
       <c r="F45" s="6">
         <v>42</v>
@@ -12240,7 +12244,7 @@
         <v>30524</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E46" s="29"/>
       <c r="F46" s="6">
         <v>43</v>
@@ -12267,7 +12271,7 @@
         <v>30570</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E47" s="29"/>
       <c r="F47" s="6">
         <v>44</v>
@@ -12294,7 +12298,7 @@
         <v>30751</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E48" s="29"/>
       <c r="F48" s="6">
         <v>45</v>
@@ -12321,7 +12325,7 @@
         <v>30509</v>
       </c>
     </row>
-    <row r="49" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E49" s="29"/>
       <c r="F49" s="6">
         <v>46</v>
@@ -12348,7 +12352,7 @@
         <v>30719</v>
       </c>
     </row>
-    <row r="50" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E50" s="29"/>
       <c r="F50" s="6">
         <v>47</v>
@@ -12375,7 +12379,7 @@
         <v>30764</v>
       </c>
     </row>
-    <row r="51" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E51" s="29"/>
       <c r="F51" s="6">
         <v>48</v>
@@ -12402,7 +12406,7 @@
         <v>30606</v>
       </c>
     </row>
-    <row r="52" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E52" s="29"/>
       <c r="F52" s="6">
         <v>49</v>
@@ -12429,7 +12433,7 @@
         <v>30589</v>
       </c>
     </row>
-    <row r="53" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E53" s="29"/>
       <c r="F53" s="6">
         <v>50</v>
@@ -12456,7 +12460,7 @@
         <v>30630</v>
       </c>
     </row>
-    <row r="54" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E54" s="29"/>
       <c r="F54" s="6">
         <v>51</v>
@@ -12483,7 +12487,7 @@
         <v>30515</v>
       </c>
     </row>
-    <row r="55" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E55" s="29"/>
       <c r="F55" s="6">
         <v>52</v>
@@ -12510,7 +12514,7 @@
         <v>30743</v>
       </c>
     </row>
-    <row r="56" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E56" s="29"/>
       <c r="F56" s="6">
         <v>53</v>
@@ -12537,7 +12541,7 @@
         <v>30609</v>
       </c>
     </row>
-    <row r="57" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E57" s="29"/>
       <c r="F57" s="6">
         <v>54</v>
@@ -12564,7 +12568,7 @@
         <v>30524</v>
       </c>
     </row>
-    <row r="58" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E58" s="29"/>
       <c r="F58" s="6">
         <v>55</v>
@@ -12591,7 +12595,7 @@
         <v>30516</v>
       </c>
     </row>
-    <row r="59" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E59" s="29"/>
       <c r="F59" s="6">
         <v>56</v>
@@ -12618,7 +12622,7 @@
         <v>30523</v>
       </c>
     </row>
-    <row r="60" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E60" s="29"/>
       <c r="F60" s="6">
         <v>57</v>
@@ -12645,7 +12649,7 @@
         <v>30670</v>
       </c>
     </row>
-    <row r="61" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E61" s="29"/>
       <c r="F61" s="6">
         <v>58</v>
@@ -12672,7 +12676,7 @@
         <v>30575</v>
       </c>
     </row>
-    <row r="62" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E62" s="29"/>
       <c r="F62" s="6">
         <v>59</v>
@@ -12699,7 +12703,7 @@
         <v>30691</v>
       </c>
     </row>
-    <row r="63" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E63" s="29"/>
       <c r="F63" s="6">
         <v>60</v>
@@ -12726,7 +12730,7 @@
         <v>30552</v>
       </c>
     </row>
-    <row r="64" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E64" s="29"/>
       <c r="F64" s="6">
         <v>61</v>
@@ -12753,7 +12757,7 @@
         <v>30645</v>
       </c>
     </row>
-    <row r="65" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E65" s="29"/>
       <c r="F65" s="6">
         <v>62</v>
@@ -12780,7 +12784,7 @@
         <v>30591</v>
       </c>
     </row>
-    <row r="66" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E66" s="29"/>
       <c r="F66" s="6">
         <v>63</v>
@@ -12807,7 +12811,7 @@
         <v>30694</v>
       </c>
     </row>
-    <row r="67" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E67" s="29"/>
       <c r="F67" s="6">
         <v>64</v>
@@ -12834,7 +12838,7 @@
         <v>30595</v>
       </c>
     </row>
-    <row r="68" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E68" s="29"/>
       <c r="F68" s="6">
         <v>65</v>
@@ -12861,7 +12865,7 @@
         <v>30661</v>
       </c>
     </row>
-    <row r="69" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E69" s="29"/>
       <c r="F69" s="6">
         <v>66</v>
@@ -12888,7 +12892,7 @@
         <v>30713</v>
       </c>
     </row>
-    <row r="70" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E70" s="29"/>
       <c r="F70" s="6">
         <v>67</v>
@@ -12915,7 +12919,7 @@
         <v>30701</v>
       </c>
     </row>
-    <row r="71" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E71" s="29"/>
       <c r="F71" s="6">
         <v>68</v>
@@ -12942,7 +12946,7 @@
         <v>30603</v>
       </c>
     </row>
-    <row r="72" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E72" s="29"/>
       <c r="F72" s="6">
         <v>69</v>
@@ -12969,7 +12973,7 @@
         <v>30585</v>
       </c>
     </row>
-    <row r="73" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E73" s="29"/>
       <c r="F73" s="6">
         <v>70</v>
@@ -12996,7 +13000,7 @@
         <v>30557</v>
       </c>
     </row>
-    <row r="74" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E74" s="29"/>
       <c r="F74" s="6">
         <v>71</v>
@@ -13023,7 +13027,7 @@
         <v>30577</v>
       </c>
     </row>
-    <row r="75" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E75" s="29"/>
       <c r="F75" s="6">
         <v>72</v>
@@ -13050,7 +13054,7 @@
         <v>30712</v>
       </c>
     </row>
-    <row r="76" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E76" s="29"/>
       <c r="F76" s="6">
         <v>73</v>
@@ -13077,7 +13081,7 @@
         <v>30521</v>
       </c>
     </row>
-    <row r="77" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E77" s="29"/>
       <c r="F77" s="6">
         <v>74</v>
@@ -13104,7 +13108,7 @@
         <v>30645</v>
       </c>
     </row>
-    <row r="78" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E78" s="29"/>
       <c r="F78" s="6">
         <v>75</v>
@@ -13131,7 +13135,7 @@
         <v>30634</v>
       </c>
     </row>
-    <row r="79" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E79" s="29"/>
       <c r="F79" s="6">
         <v>76</v>
@@ -13158,7 +13162,7 @@
         <v>30658</v>
       </c>
     </row>
-    <row r="80" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E80" s="29"/>
       <c r="F80" s="6">
         <v>77</v>
@@ -13185,7 +13189,7 @@
         <v>30585</v>
       </c>
     </row>
-    <row r="81" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E81" s="29"/>
       <c r="F81" s="6">
         <v>78</v>
@@ -13212,7 +13216,7 @@
         <v>30697</v>
       </c>
     </row>
-    <row r="82" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E82" s="29"/>
       <c r="F82" s="6">
         <v>79</v>
@@ -13239,7 +13243,7 @@
         <v>30690</v>
       </c>
     </row>
-    <row r="83" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E83" s="29"/>
       <c r="F83" s="6">
         <v>80</v>
@@ -13266,7 +13270,7 @@
         <v>30580</v>
       </c>
     </row>
-    <row r="84" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E84" s="29"/>
       <c r="F84" s="6">
         <v>81</v>
@@ -13293,7 +13297,7 @@
         <v>30756</v>
       </c>
     </row>
-    <row r="85" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E85" s="29"/>
       <c r="F85" s="6">
         <v>82</v>
@@ -13320,7 +13324,7 @@
         <v>30767</v>
       </c>
     </row>
-    <row r="86" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E86" s="29"/>
       <c r="F86" s="6">
         <v>83</v>
@@ -13347,7 +13351,7 @@
         <v>30703</v>
       </c>
     </row>
-    <row r="87" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E87" s="29"/>
       <c r="F87" s="6">
         <v>84</v>
@@ -13374,7 +13378,7 @@
         <v>30767</v>
       </c>
     </row>
-    <row r="88" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E88" s="29"/>
       <c r="F88" s="6">
         <v>85</v>
@@ -13401,7 +13405,7 @@
         <v>30578</v>
       </c>
     </row>
-    <row r="89" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E89" s="29"/>
       <c r="F89" s="6">
         <v>86</v>
@@ -13428,7 +13432,7 @@
         <v>30506</v>
       </c>
     </row>
-    <row r="90" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E90" s="29"/>
       <c r="F90" s="6">
         <v>87</v>
@@ -13455,7 +13459,7 @@
         <v>30733</v>
       </c>
     </row>
-    <row r="91" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E91" s="29"/>
       <c r="F91" s="6">
         <v>88</v>
@@ -13482,7 +13486,7 @@
         <v>30742</v>
       </c>
     </row>
-    <row r="92" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E92" s="29"/>
       <c r="F92" s="6">
         <v>89</v>
@@ -13509,7 +13513,7 @@
         <v>30637</v>
       </c>
     </row>
-    <row r="93" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E93" s="29"/>
       <c r="F93" s="6">
         <v>90</v>
@@ -13536,7 +13540,7 @@
         <v>30565</v>
       </c>
     </row>
-    <row r="94" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E94" s="29"/>
       <c r="F94" s="6">
         <v>91</v>
@@ -13563,7 +13567,7 @@
         <v>30712</v>
       </c>
     </row>
-    <row r="95" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E95" s="29"/>
       <c r="F95" s="6">
         <v>92</v>
@@ -13590,7 +13594,7 @@
         <v>30758</v>
       </c>
     </row>
-    <row r="96" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E96" s="29"/>
       <c r="F96" s="6">
         <v>93</v>
@@ -13617,7 +13621,7 @@
         <v>30562</v>
       </c>
     </row>
-    <row r="97" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E97" s="29"/>
       <c r="F97" s="6">
         <v>94</v>
@@ -13644,7 +13648,7 @@
         <v>30694</v>
       </c>
     </row>
-    <row r="98" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E98" s="29"/>
       <c r="F98" s="6">
         <v>95</v>
@@ -13671,7 +13675,7 @@
         <v>30706</v>
       </c>
     </row>
-    <row r="99" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E99" s="29"/>
       <c r="F99" s="6">
         <v>96</v>
@@ -13698,7 +13702,7 @@
         <v>30512</v>
       </c>
     </row>
-    <row r="100" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E100" s="29"/>
       <c r="F100" s="6">
         <v>97</v>
@@ -13725,7 +13729,7 @@
         <v>30630</v>
       </c>
     </row>
-    <row r="101" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E101" s="29"/>
       <c r="F101" s="6">
         <v>98</v>
@@ -13752,7 +13756,7 @@
         <v>30550</v>
       </c>
     </row>
-    <row r="102" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E102" s="29"/>
       <c r="F102" s="6">
         <v>99</v>
@@ -13779,7 +13783,7 @@
         <v>30573</v>
       </c>
     </row>
-    <row r="103" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E103" s="29"/>
       <c r="F103" s="6">
         <v>100</v>
@@ -13806,7 +13810,7 @@
         <v>30545</v>
       </c>
     </row>
-    <row r="104" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G104" s="19"/>
       <c r="H104" s="19"/>
       <c r="I104" s="19"/>
@@ -13830,61 +13834,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="19"/>
-    <col min="9" max="9" width="9.140625" style="19" customWidth="1"/>
-    <col min="10" max="15" width="9.140625" style="19"/>
-    <col min="16" max="16" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="19" customWidth="1"/>
-    <col min="18" max="22" width="9.140625" style="19"/>
-    <col min="23" max="23" width="9.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="16.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" style="19"/>
+    <col min="9" max="9" width="9.109375" style="19" customWidth="1"/>
+    <col min="10" max="15" width="9.109375" style="19"/>
+    <col min="16" max="16" width="16.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="19" customWidth="1"/>
+    <col min="18" max="22" width="9.109375" style="19"/>
+    <col min="23" max="23" width="9.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="43"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
       <c r="N1" s="17"/>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
       <c r="W1" s="17"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -13944,7 +13948,7 @@
       </c>
       <c r="W2" s="23"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>64</v>
       </c>
@@ -13958,30 +13962,30 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
       <c r="N3" s="17"/>
       <c r="P3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="Q3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="45"/>
       <c r="W3" s="17"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>128</v>
       </c>
@@ -14039,7 +14043,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>256</v>
       </c>
@@ -14048,10 +14052,10 @@
         <v>285.48</v>
       </c>
       <c r="C5"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="37"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="6">
         <v>2</v>
       </c>
@@ -14099,7 +14103,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>512</v>
       </c>
@@ -14161,7 +14165,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1024</v>
       </c>
@@ -14224,7 +14228,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2048</v>
       </c>
@@ -14287,7 +14291,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>4096</v>
       </c>
@@ -14350,7 +14354,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="7"/>
       <c r="C10"/>
@@ -14408,7 +14412,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -14466,11 +14470,11 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="37"/>
+      <c r="B12" s="43"/>
       <c r="D12" s="6">
         <v>2048</v>
       </c>
@@ -14525,7 +14529,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
@@ -14586,7 +14590,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
         <v>1</v>
       </c>
@@ -14641,7 +14645,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>2</v>
       </c>
@@ -14697,7 +14701,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>4</v>
       </c>
@@ -14706,10 +14710,10 @@
         <v>1051.98</v>
       </c>
       <c r="C16"/>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="37"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="6">
         <v>13</v>
       </c>
@@ -14757,7 +14761,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>8</v>
       </c>
@@ -14819,7 +14823,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -14882,7 +14886,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>32</v>
       </c>
@@ -14945,7 +14949,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="7"/>
       <c r="C20"/>
@@ -15003,7 +15007,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C21"/>
       <c r="D21" s="16">
         <v>8</v>
@@ -15059,12 +15063,12 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="42"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="6">
         <v>16</v>
       </c>
@@ -15119,11 +15123,11 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="6">
@@ -15180,12 +15184,12 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f>A3/B24</f>
         <v>8</v>
       </c>
-      <c r="B24" s="46">
+      <c r="B24" s="48">
         <v>8</v>
       </c>
       <c r="D24" s="10"/>
@@ -15237,12 +15241,12 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f>A4/B24</f>
         <v>16</v>
       </c>
-      <c r="B25" s="44"/>
+      <c r="B25" s="49"/>
       <c r="E25" s="1"/>
       <c r="F25" s="6">
         <v>22</v>
@@ -15291,12 +15295,12 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f>A5/B24</f>
         <v>32</v>
       </c>
-      <c r="B26" s="44"/>
+      <c r="B26" s="49"/>
       <c r="E26" s="1"/>
       <c r="F26" s="6">
         <v>23</v>
@@ -15345,12 +15349,12 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f>A6/B24</f>
         <v>64</v>
       </c>
-      <c r="B27" s="44"/>
+      <c r="B27" s="49"/>
       <c r="E27" s="1"/>
       <c r="F27" s="6">
         <v>24</v>
@@ -15399,12 +15403,12 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f>A7/B24</f>
         <v>128</v>
       </c>
-      <c r="B28" s="44"/>
+      <c r="B28" s="49"/>
       <c r="E28" s="1"/>
       <c r="F28" s="6">
         <v>25</v>
@@ -15453,12 +15457,12 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f>A8/B24</f>
         <v>256</v>
       </c>
-      <c r="B29" s="44"/>
+      <c r="B29" s="49"/>
       <c r="E29" s="1"/>
       <c r="F29" s="6">
         <v>26</v>
@@ -15507,12 +15511,12 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <f>A9/B24</f>
         <v>512</v>
       </c>
-      <c r="B30" s="44"/>
+      <c r="B30" s="49"/>
       <c r="F30" s="6">
         <v>27</v>
       </c>
@@ -15560,7 +15564,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
       <c r="F31" s="6">
         <v>28</v>
@@ -15609,12 +15613,12 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A32" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
       <c r="E32" s="1"/>
       <c r="F32" s="6">
         <v>29</v>
@@ -15663,7 +15667,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>9</v>
       </c>
@@ -15721,7 +15725,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>64</v>
       </c>
@@ -15781,7 +15785,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>128</v>
       </c>
@@ -15841,7 +15845,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>256</v>
       </c>
@@ -15901,7 +15905,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>512</v>
       </c>
@@ -15961,7 +15965,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>1024</v>
       </c>
@@ -16021,7 +16025,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>2048</v>
       </c>
@@ -16079,7 +16083,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>4096</v>
       </c>
@@ -16137,7 +16141,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F41" s="6">
         <v>38</v>
       </c>
@@ -16184,11 +16188,11 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="48" t="s">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B42" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="48"/>
+      <c r="C42" s="46"/>
       <c r="F42" s="6">
         <v>39</v>
       </c>
@@ -16235,7 +16239,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
         <v>26</v>
       </c>
@@ -16288,12 +16292,12 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B44" s="16">
         <f>('Seq. Results'!B3+'Seq. Results'!E13)/(B3-E7) - B34</f>
         <v>1.7444756998069771E-2</v>
       </c>
-      <c r="C44" s="49">
+      <c r="C44" s="42">
         <f>B34-('Seq. Results'!B3-'Seq. Results'!E13)/(B3+E7)</f>
         <v>1.6003102759232612E-2</v>
       </c>
@@ -16343,12 +16347,12 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B45" s="16">
         <f>('Seq. Results'!B4+'Seq. Results'!E14)/(B4-E8) - B35</f>
         <v>2.9219082494406301E-2</v>
       </c>
-      <c r="C45" s="49">
+      <c r="C45" s="42">
         <f>B35-('Seq. Results'!B4-'Seq. Results'!E14)/(B4+E8)</f>
         <v>2.7451846608023744E-2</v>
       </c>
@@ -16398,12 +16402,12 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B46" s="16">
         <f>('Seq. Results'!B5+'Seq. Results'!E15)/(B5-E9) - B36</f>
         <v>2.9908795413046141E-2</v>
       </c>
-      <c r="C46" s="49">
+      <c r="C46" s="42">
         <f>B36-('Seq. Results'!B5-'Seq. Results'!E15)/(B5+E9)</f>
         <v>2.9045166356023167E-2</v>
       </c>
@@ -16453,12 +16457,12 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B47" s="16">
         <f>('Seq. Results'!B6+'Seq. Results'!E16)/(B6-E10) - B37</f>
         <v>3.870168981476052E-2</v>
       </c>
-      <c r="C47" s="49">
+      <c r="C47" s="42">
         <f>B37-('Seq. Results'!B6-'Seq. Results'!E16)/(B6+E10)</f>
         <v>3.7978282803384555E-2</v>
       </c>
@@ -16508,12 +16512,12 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B48" s="16">
         <f>('Seq. Results'!B7+'Seq. Results'!E17)/(B7-E11) - B38</f>
         <v>3.855226750576346E-2</v>
       </c>
-      <c r="C48" s="49">
+      <c r="C48" s="42">
         <f>B38-('Seq. Results'!B7-'Seq. Results'!E17)/(B7+E11)</f>
         <v>3.8208409174706581E-2</v>
       </c>
@@ -16563,12 +16567,12 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B49" s="16">
         <f>('Seq. Results'!B8+'Seq. Results'!E18)/(B8-E12) - B39</f>
         <v>5.5918063938335649E-2</v>
       </c>
-      <c r="C49" s="49">
+      <c r="C49" s="42">
         <f>B39-('Seq. Results'!B8-'Seq. Results'!E18)/(B8+E12)</f>
         <v>5.5331335328913767E-2</v>
       </c>
@@ -16618,12 +16622,12 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B50" s="16">
         <f>('Seq. Results'!B9+'Seq. Results'!E19)/(B9-E13) - B40</f>
         <v>6.1641128484716035E-2</v>
       </c>
-      <c r="C50" s="49">
+      <c r="C50" s="42">
         <f>B40-('Seq. Results'!B9-'Seq. Results'!E19)/(B9+E13)</f>
         <v>6.1166544585375959E-2</v>
       </c>
@@ -16673,7 +16677,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F51" s="6">
         <v>48</v>
       </c>
@@ -16720,7 +16724,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F52" s="6">
         <v>49</v>
       </c>
@@ -16767,7 +16771,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F53" s="6">
         <v>50</v>
       </c>
@@ -16814,7 +16818,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F54" s="6">
         <v>51</v>
       </c>
@@ -16861,7 +16865,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F55" s="6">
         <v>52</v>
       </c>
@@ -16908,7 +16912,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F56" s="6">
         <v>53</v>
       </c>
@@ -16955,7 +16959,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F57" s="6">
         <v>54</v>
       </c>
@@ -17002,7 +17006,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F58" s="6">
         <v>55</v>
       </c>
@@ -17049,7 +17053,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F59" s="6">
         <v>56</v>
       </c>
@@ -17096,7 +17100,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F60" s="6">
         <v>57</v>
       </c>
@@ -17143,7 +17147,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F61" s="6">
         <v>58</v>
       </c>
@@ -17190,7 +17194,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="62" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F62" s="6">
         <v>59</v>
       </c>
@@ -17237,7 +17241,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F63" s="6">
         <v>60</v>
       </c>
@@ -17284,7 +17288,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F64" s="6">
         <v>61</v>
       </c>
@@ -17331,7 +17335,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="65" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F65" s="6">
         <v>62</v>
       </c>
@@ -17378,7 +17382,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="66" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F66" s="6">
         <v>63</v>
       </c>
@@ -17425,7 +17429,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="67" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F67" s="6">
         <v>64</v>
       </c>
@@ -17472,7 +17476,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="68" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F68" s="6">
         <v>65</v>
       </c>
@@ -17519,7 +17523,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="69" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F69" s="6">
         <v>66</v>
       </c>
@@ -17566,7 +17570,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="70" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F70" s="6">
         <v>67</v>
       </c>
@@ -17613,7 +17617,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="71" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F71" s="6">
         <v>68</v>
       </c>
@@ -17660,7 +17664,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="72" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F72" s="6">
         <v>69</v>
       </c>
@@ -17707,7 +17711,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="73" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F73" s="6">
         <v>70</v>
       </c>
@@ -17754,7 +17758,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="74" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F74" s="6">
         <v>71</v>
       </c>
@@ -17801,7 +17805,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="75" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F75" s="6">
         <v>72</v>
       </c>
@@ -17848,7 +17852,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="76" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F76" s="6">
         <v>73</v>
       </c>
@@ -17895,7 +17899,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="77" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F77" s="6">
         <v>74</v>
       </c>
@@ -17942,7 +17946,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="78" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F78" s="6">
         <v>75</v>
       </c>
@@ -17989,7 +17993,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="79" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F79" s="6">
         <v>76</v>
       </c>
@@ -18036,7 +18040,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="80" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F80" s="6">
         <v>77</v>
       </c>
@@ -18083,7 +18087,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="81" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F81" s="6">
         <v>78</v>
       </c>
@@ -18130,7 +18134,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="82" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F82" s="6">
         <v>79</v>
       </c>
@@ -18177,7 +18181,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="83" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F83" s="6">
         <v>80</v>
       </c>
@@ -18224,7 +18228,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="84" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F84" s="6">
         <v>81</v>
       </c>
@@ -18271,7 +18275,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="85" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F85" s="6">
         <v>82</v>
       </c>
@@ -18318,7 +18322,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="86" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F86" s="6">
         <v>83</v>
       </c>
@@ -18365,7 +18369,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="87" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F87" s="6">
         <v>84</v>
       </c>
@@ -18412,7 +18416,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="88" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F88" s="6">
         <v>85</v>
       </c>
@@ -18459,7 +18463,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="89" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F89" s="6">
         <v>86</v>
       </c>
@@ -18506,7 +18510,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="90" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F90" s="6">
         <v>87</v>
       </c>
@@ -18553,7 +18557,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="91" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F91" s="6">
         <v>88</v>
       </c>
@@ -18600,7 +18604,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="92" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F92" s="6">
         <v>89</v>
       </c>
@@ -18647,7 +18651,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="93" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F93" s="6">
         <v>90</v>
       </c>
@@ -18694,7 +18698,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="94" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F94" s="6">
         <v>91</v>
       </c>
@@ -18741,7 +18745,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="95" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F95" s="6">
         <v>92</v>
       </c>
@@ -18788,7 +18792,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="96" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F96" s="6">
         <v>93</v>
       </c>
@@ -18835,7 +18839,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="97" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F97" s="6">
         <v>94</v>
       </c>
@@ -18882,7 +18886,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="98" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F98" s="6">
         <v>95</v>
       </c>
@@ -18929,7 +18933,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="99" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F99" s="6">
         <v>96</v>
       </c>
@@ -18976,7 +18980,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="100" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F100" s="6">
         <v>97</v>
       </c>
@@ -19023,7 +19027,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="101" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F101" s="6">
         <v>98</v>
       </c>
@@ -19070,7 +19074,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="102" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F102" s="6">
         <v>99</v>
       </c>
@@ -19117,7 +19121,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="103" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F103" s="6">
         <v>100</v>
       </c>
@@ -19166,6 +19170,10 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="Q3:V3"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G1:M1"/>
@@ -19174,10 +19182,6 @@
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="Q3:V3"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19191,28 +19195,28 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
@@ -19221,7 +19225,7 @@
       </c>
       <c r="D2" s="14"/>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
@@ -19237,7 +19241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
@@ -19297,7 +19301,7 @@
       <c r="BA4" s="1"/>
       <c r="BB4" s="1"/>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>20</v>
       </c>
@@ -19356,7 +19360,7 @@
       <c r="BA5" s="1"/>
       <c r="BB5" s="1"/>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B6" s="29"/>
       <c r="C6" s="18"/>
       <c r="H6">
@@ -19410,7 +19414,7 @@
       <c r="BA6" s="1"/>
       <c r="BB6" s="1"/>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
       <c r="H7">
         <v>1270</v>
       </c>
@@ -19462,11 +19466,11 @@
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="B8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="43"/>
       <c r="H8">
         <v>1268</v>
       </c>
@@ -19518,7 +19522,7 @@
       <c r="BA8" s="1"/>
       <c r="BB8" s="1"/>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
@@ -19576,7 +19580,7 @@
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>7</v>
       </c>
@@ -19637,7 +19641,7 @@
       <c r="BA10" s="1"/>
       <c r="BB10" s="1"/>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
@@ -19698,7 +19702,7 @@
       <c r="BA11" s="1"/>
       <c r="BB11" s="1"/>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
@@ -19759,7 +19763,7 @@
       <c r="BA12" s="1"/>
       <c r="BB12" s="1"/>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
       <c r="C13" s="30"/>
       <c r="D13" s="17"/>
@@ -19815,7 +19819,7 @@
       <c r="BA13" s="1"/>
       <c r="BB13" s="1"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="30"/>
       <c r="D14" s="17"/>
@@ -19871,7 +19875,7 @@
       <c r="BA14" s="1"/>
       <c r="BB14" s="1"/>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="30"/>
       <c r="D15" s="17"/>
@@ -19926,7 +19930,7 @@
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
       <c r="C16" s="30"/>
       <c r="H16">
@@ -19980,7 +19984,7 @@
       <c r="BA16" s="1"/>
       <c r="BB16" s="1"/>
     </row>
-    <row r="17" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H17">
         <v>1278</v>
       </c>
@@ -20032,7 +20036,7 @@
       <c r="BA17" s="1"/>
       <c r="BB17" s="1"/>
     </row>
-    <row r="18" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H18">
         <v>1271</v>
       </c>
@@ -20084,7 +20088,7 @@
       <c r="BA18" s="1"/>
       <c r="BB18" s="1"/>
     </row>
-    <row r="19" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B19" s="29"/>
       <c r="H19">
         <v>1267</v>
@@ -20137,7 +20141,7 @@
       <c r="BA19" s="1"/>
       <c r="BB19" s="1"/>
     </row>
-    <row r="20" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B20" s="14"/>
       <c r="H20">
         <v>1265</v>
@@ -20190,7 +20194,7 @@
       <c r="BA20" s="1"/>
       <c r="BB20" s="1"/>
     </row>
-    <row r="21" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B21" s="14"/>
       <c r="H21">
         <v>1269</v>
@@ -20243,7 +20247,7 @@
       <c r="BA21" s="1"/>
       <c r="BB21" s="1"/>
     </row>
-    <row r="22" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B22" s="14"/>
       <c r="H22">
         <v>1276</v>
@@ -20296,7 +20300,7 @@
       <c r="BA22" s="1"/>
       <c r="BB22" s="1"/>
     </row>
-    <row r="23" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="H23">
         <v>1272</v>
@@ -20349,7 +20353,7 @@
       <c r="BA23" s="1"/>
       <c r="BB23" s="1"/>
     </row>
-    <row r="24" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H24">
         <v>1281</v>
       </c>
@@ -20401,7 +20405,7 @@
       <c r="BA24" s="1"/>
       <c r="BB24" s="1"/>
     </row>
-    <row r="25" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H25">
         <v>1267</v>
       </c>
@@ -20453,7 +20457,7 @@
       <c r="BA25" s="1"/>
       <c r="BB25" s="1"/>
     </row>
-    <row r="26" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H26">
         <v>1276</v>
       </c>
@@ -20505,7 +20509,7 @@
       <c r="BA26" s="1"/>
       <c r="BB26" s="1"/>
     </row>
-    <row r="27" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H27">
         <v>1283</v>
       </c>
@@ -20557,7 +20561,7 @@
       <c r="BA27" s="1"/>
       <c r="BB27" s="1"/>
     </row>
-    <row r="28" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H28">
         <v>1298</v>
       </c>
@@ -20609,7 +20613,7 @@
       <c r="BA28" s="1"/>
       <c r="BB28" s="1"/>
     </row>
-    <row r="29" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H29">
         <v>1273</v>
       </c>
@@ -20661,7 +20665,7 @@
       <c r="BA29" s="1"/>
       <c r="BB29" s="1"/>
     </row>
-    <row r="30" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H30">
         <v>1265</v>
       </c>
@@ -20713,7 +20717,7 @@
       <c r="BA30" s="1"/>
       <c r="BB30" s="1"/>
     </row>
-    <row r="31" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H31">
         <v>1266</v>
       </c>
@@ -20765,7 +20769,7 @@
       <c r="BA31" s="1"/>
       <c r="BB31" s="1"/>
     </row>
-    <row r="32" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:54" x14ac:dyDescent="0.3">
       <c r="H32">
         <v>1272</v>
       </c>
@@ -20817,7 +20821,7 @@
       <c r="BA32" s="1"/>
       <c r="BB32" s="1"/>
     </row>
-    <row r="33" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H33">
         <v>1270</v>
       </c>
@@ -20869,7 +20873,7 @@
       <c r="BA33" s="1"/>
       <c r="BB33" s="1"/>
     </row>
-    <row r="34" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H34">
         <v>1274</v>
       </c>
@@ -20921,7 +20925,7 @@
       <c r="BA34" s="1"/>
       <c r="BB34" s="1"/>
     </row>
-    <row r="35" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H35">
         <v>1291</v>
       </c>
@@ -20973,7 +20977,7 @@
       <c r="BA35" s="1"/>
       <c r="BB35" s="1"/>
     </row>
-    <row r="36" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H36">
         <v>1275</v>
       </c>
@@ -21025,7 +21029,7 @@
       <c r="BA36" s="1"/>
       <c r="BB36" s="1"/>
     </row>
-    <row r="37" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H37">
         <v>1271</v>
       </c>
@@ -21077,7 +21081,7 @@
       <c r="BA37" s="1"/>
       <c r="BB37" s="1"/>
     </row>
-    <row r="38" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H38">
         <v>1280</v>
       </c>
@@ -21129,7 +21133,7 @@
       <c r="BA38" s="1"/>
       <c r="BB38" s="1"/>
     </row>
-    <row r="39" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H39">
         <v>1269</v>
       </c>
@@ -21181,7 +21185,7 @@
       <c r="BA39" s="1"/>
       <c r="BB39" s="1"/>
     </row>
-    <row r="40" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H40">
         <v>1275</v>
       </c>
@@ -21233,7 +21237,7 @@
       <c r="BA40" s="1"/>
       <c r="BB40" s="1"/>
     </row>
-    <row r="41" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H41">
         <v>1269</v>
       </c>
@@ -21285,7 +21289,7 @@
       <c r="BA41" s="1"/>
       <c r="BB41" s="1"/>
     </row>
-    <row r="42" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H42">
         <v>1281</v>
       </c>
@@ -21337,7 +21341,7 @@
       <c r="BA42" s="1"/>
       <c r="BB42" s="1"/>
     </row>
-    <row r="43" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H43">
         <v>1267</v>
       </c>
@@ -21389,7 +21393,7 @@
       <c r="BA43" s="1"/>
       <c r="BB43" s="1"/>
     </row>
-    <row r="44" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H44">
         <v>1261</v>
       </c>
@@ -21441,7 +21445,7 @@
       <c r="BA44" s="1"/>
       <c r="BB44" s="1"/>
     </row>
-    <row r="45" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H45">
         <v>1273</v>
       </c>
@@ -21493,7 +21497,7 @@
       <c r="BA45" s="1"/>
       <c r="BB45" s="1"/>
     </row>
-    <row r="46" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H46">
         <v>1267</v>
       </c>
@@ -21545,7 +21549,7 @@
       <c r="BA46" s="1"/>
       <c r="BB46" s="1"/>
     </row>
-    <row r="47" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H47">
         <v>1267</v>
       </c>
@@ -21597,7 +21601,7 @@
       <c r="BA47" s="1"/>
       <c r="BB47" s="1"/>
     </row>
-    <row r="48" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H48">
         <v>1265</v>
       </c>
@@ -21649,7 +21653,7 @@
       <c r="BA48" s="1"/>
       <c r="BB48" s="1"/>
     </row>
-    <row r="49" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H49">
         <v>1279</v>
       </c>
@@ -21701,7 +21705,7 @@
       <c r="BA49" s="1"/>
       <c r="BB49" s="1"/>
     </row>
-    <row r="50" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H50">
         <v>1270</v>
       </c>
@@ -21753,7 +21757,7 @@
       <c r="BA50" s="1"/>
       <c r="BB50" s="1"/>
     </row>
-    <row r="51" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H51">
         <v>1277</v>
       </c>
@@ -21805,7 +21809,7 @@
       <c r="BA51" s="1"/>
       <c r="BB51" s="1"/>
     </row>
-    <row r="52" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H52">
         <v>1269</v>
       </c>
@@ -21857,7 +21861,7 @@
       <c r="BA52" s="1"/>
       <c r="BB52" s="1"/>
     </row>
-    <row r="53" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:54" x14ac:dyDescent="0.3">
       <c r="H53">
         <v>1267</v>
       </c>
@@ -21909,7 +21913,7 @@
       <c r="BA53" s="1"/>
       <c r="BB53" s="1"/>
     </row>
-    <row r="54" spans="8:54" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:54" x14ac:dyDescent="0.3">
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>

</xml_diff>

<commit_message>
Kicked out glab, relocate safety commit.
</commit_message>
<xml_diff>
--- a/Coursework Part 2/results.xlsx
+++ b/Coursework Part 2/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Seq. Results" sheetId="1" r:id="rId1"/>
@@ -2034,7 +2034,7 @@
           <c:x val="9.253226288333459E-2"/>
           <c:y val="0.10236975533648379"/>
           <c:w val="0.90746773711666529"/>
-          <c:h val="0.7010473522718641"/>
+          <c:h val="0.73544453437167423"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2737,6 +2737,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28237827003234861"/>
+          <c:y val="0.94181780814060934"/>
+          <c:w val="0.42937522554138019"/>
+          <c:h val="5.6158829189953928E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6562,7 +6572,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0"/>
+    <sheetView zoomScale="97" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10498,7 +10508,7 @@
   <dimension ref="A1:V104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B9"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13834,8 +13844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Katherine nearly spilled pickles on my laptop safety commit.
</commit_message>
<xml_diff>
--- a/Coursework Part 2/results.xlsx
+++ b/Coursework Part 2/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Seq. Results" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,16 @@
     <sheet name="Comparison 1" sheetId="13" r:id="rId5"/>
     <sheet name="Comparison 2" sheetId="12" r:id="rId6"/>
     <sheet name="Comaprison 3" sheetId="7" r:id="rId7"/>
-    <sheet name="Comparison 4" sheetId="15" r:id="rId8"/>
-    <sheet name="Seq Graph" sheetId="14" r:id="rId9"/>
+    <sheet name="Comparison 4" sheetId="17" r:id="rId8"/>
+    <sheet name="Comparison 5" sheetId="16" r:id="rId9"/>
+    <sheet name="Seq Graph" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
   <si>
     <t>Time / ms</t>
   </si>
@@ -111,6 +112,9 @@
   </si>
   <si>
     <t>Neg</t>
+  </si>
+  <si>
+    <t>Efficiency Err</t>
   </si>
 </sst>
 </file>
@@ -723,7 +727,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -839,6 +843,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -859,6 +866,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2838,7 +2851,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" sz="2400" baseline="0"/>
-              <a:t>Parallel Speedups Comparison</a:t>
+              <a:t>Parallel Speedup Comparison</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3045,7 +3058,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4928-43A8-8771-5982C00D3F1D}"/>
+              <c16:uniqueId val="{00000000-FE52-4798-BDFB-174F74A7828B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3205,7 +3218,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4928-43A8-8771-5982C00D3F1D}"/>
+              <c16:uniqueId val="{00000001-FE52-4798-BDFB-174F74A7828B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3331,6 +3344,7 @@
         <c:axId val="507078200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="12"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3403,7 +3417,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3443,6 +3457,7 @@
         <c:crossAx val="507077544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3511,6 +3526,715 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2400" baseline="0"/>
+              <a:t>Parallel Efficiency Comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.253226288333459E-2"/>
+          <c:y val="0.10236975533648379"/>
+          <c:w val="0.90746773711666529"/>
+          <c:h val="0.7010473522718641"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>OpenMP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>OMP!$D$35:$D$41</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.17564529666854584</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.0414514330976981E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.1461287737949641E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.140490403233807E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.8558105772825728E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.7632460421516134E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.662473591188208E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>OMP!$E$35:$E$41</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>9.0646185797987194E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.5682745159775431E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.0331018257214062E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.1126111413843898E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.757985789725085E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.7297527925893581E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.6481024280428089E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>OMP!$A$24:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>OMP!$C$24:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.32972186287192756</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.44133376991923162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54311852549441675</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60388168496795713</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63744203883833628</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64567980092097066</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65948489909056629</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8655-43DC-8650-DF6CD386C93D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CUDA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>CUDA!$D$44:$D$50</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>2.1805946247587214E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.8261926559003938E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.346498566576919E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.0471390335563313E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.0118958988877703E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.1842993725912363E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.2039282907171101E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>CUDA!$E$44:$E$51</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>2.0003878449040766E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.715740413001484E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.0766144862572395E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.9341066880288368E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.9850319667739517E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.161380286285694E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.1946590739331242E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>OMP!$A$24:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CUDA!$C$34:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.41016548463357E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.223659034377193E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5352739246181868E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8122645928757991E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7612570648698468E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2889261025396237E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3131569125467596E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8655-43DC-8650-DF6CD386C93D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="507077544"/>
+        <c:axId val="507078200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="507077544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" baseline="0"/>
+                  <a:t>Number of Bodies</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507078200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="507078200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" baseline="0"/>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507077544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3988,6 +4712,46 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6066,6 +6830,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6606,6 +7886,18 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6614,7 +7906,7 @@
 </chartsheet>
 </file>
 
-<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -6734,7 +8026,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9DAB54E-FC27-41D5-9F41-2A2F543EE98B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6758,6 +8050,39 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656948" cy="6276680"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{866F8B09-F834-4603-A81E-D46D545EFEF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -7081,32 +8406,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="44"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
       <c r="N1" s="17"/>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
       <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -7183,27 +8508,27 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
       <c r="N3" s="17"/>
       <c r="P3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="Q3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
       <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -7611,10 +8936,10 @@
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -7663,10 +8988,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="43"/>
+      <c r="B12" s="44"/>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
@@ -10507,8 +11832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10516,8 +11841,8 @@
     <col min="1" max="1" width="17.5546875" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.109375" style="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" style="17" bestFit="1" customWidth="1"/>
     <col min="7" max="14" width="9.109375" style="17"/>
     <col min="15" max="15" width="12.33203125" style="17" bestFit="1" customWidth="1"/>
@@ -10531,23 +11856,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="44"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
       <c r="Q1" s="19"/>
       <c r="R1" s="19"/>
       <c r="S1" s="19"/>
@@ -10615,15 +11940,15 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
       <c r="O3" s="10"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="19"/>
@@ -10947,10 +12272,10 @@
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -11427,11 +12752,11 @@
       <c r="V21" s="19"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
       <c r="D22"/>
       <c r="E22" s="1"/>
       <c r="F22" s="6">
@@ -11838,11 +13163,14 @@
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="E33" s="29"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="47"/>
       <c r="F33" s="6">
         <v>30</v>
       </c>
@@ -11875,7 +13203,12 @@
       <c r="C34" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="D34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="43" t="s">
+        <v>27</v>
+      </c>
       <c r="F34" s="6">
         <v>31</v>
       </c>
@@ -11910,7 +13243,14 @@
         <f>B24-('Seq. Results'!B3-'Seq. Results'!E13)/(B3+E13)</f>
         <v>0.36258474319194878</v>
       </c>
-      <c r="E35" s="29"/>
+      <c r="D35" s="16">
+        <f>((B24+B35)/B20) - C24</f>
+        <v>0.17564529666854584</v>
+      </c>
+      <c r="E35" s="42">
+        <f>C24-((B24-C35)/B20)</f>
+        <v>9.0646185797987194E-2</v>
+      </c>
       <c r="F35" s="6">
         <v>32</v>
       </c>
@@ -11945,7 +13285,14 @@
         <f>B25-('Seq. Results'!B4-'Seq. Results'!E14)/(B4+E14)</f>
         <v>0.14273098063910172</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="D36" s="16">
+        <f>((B25+B36)/B20) - C25</f>
+        <v>4.0414514330976981E-2</v>
+      </c>
+      <c r="E36" s="42">
+        <f>C25-((B25-C36)/B20)</f>
+        <v>3.5682745159775431E-2</v>
+      </c>
       <c r="F36" s="6">
         <v>33</v>
       </c>
@@ -11980,7 +13327,14 @@
         <f>B26-('Seq. Results'!B5-'Seq. Results'!E15)/(B5+E15)</f>
         <v>8.1324073028856247E-2</v>
       </c>
-      <c r="E37" s="29"/>
+      <c r="D37" s="16">
+        <f>((B26+B37)/B20) - C26</f>
+        <v>2.1461287737949641E-2</v>
+      </c>
+      <c r="E37" s="42">
+        <f>C26-((B26-C37)/B20)</f>
+        <v>2.0331018257214062E-2</v>
+      </c>
       <c r="F37" s="6">
         <v>34</v>
       </c>
@@ -12015,7 +13369,14 @@
         <f>B27-('Seq. Results'!B6-'Seq. Results'!E16)/(B6+E16)</f>
         <v>4.4504445655375591E-2</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="D38" s="16">
+        <f>((B27+B38)/B20) - C27</f>
+        <v>1.140490403233807E-2</v>
+      </c>
+      <c r="E38" s="42">
+        <f>C27-((B27-C38)/B20)</f>
+        <v>1.1126111413843898E-2</v>
+      </c>
       <c r="F38" s="6">
         <v>35</v>
       </c>
@@ -12050,7 +13411,14 @@
         <f>B28-('Seq. Results'!B7-'Seq. Results'!E17)/(B7+E17)</f>
         <v>2.703194315890034E-2</v>
       </c>
-      <c r="E39" s="29"/>
+      <c r="D39" s="16">
+        <f>((B28+B39)/B20) - C28</f>
+        <v>6.8558105772825728E-3</v>
+      </c>
+      <c r="E39" s="42">
+        <f>C28-((B28-C39)/B20)</f>
+        <v>6.757985789725085E-3</v>
+      </c>
       <c r="F39" s="6">
         <v>36</v>
       </c>
@@ -12085,7 +13453,14 @@
         <f>B29-('Seq. Results'!B8-'Seq. Results'!E18)/(B8+E18)</f>
         <v>1.4919011170357432E-2</v>
       </c>
-      <c r="E40" s="29"/>
+      <c r="D40" s="16">
+        <f>((B29+B40)/B20) - C29</f>
+        <v>3.7632460421516134E-3</v>
+      </c>
+      <c r="E40" s="42">
+        <f>C29-((B29-C40)/B20)</f>
+        <v>3.7297527925893581E-3</v>
+      </c>
       <c r="F40" s="6">
         <v>37</v>
       </c>
@@ -12120,7 +13495,14 @@
         <f>B30-('Seq. Results'!B9-'Seq. Results'!E19)/(B9+E19)</f>
         <v>1.0592409712171236E-2</v>
       </c>
-      <c r="E41" s="29"/>
+      <c r="D41" s="16">
+        <f>((B30+B41)/B20) - C30</f>
+        <v>2.662473591188208E-3</v>
+      </c>
+      <c r="E41" s="42">
+        <f>C30-((B30-C41)/B20)</f>
+        <v>2.6481024280428089E-3</v>
+      </c>
       <c r="F41" s="6">
         <v>38</v>
       </c>
@@ -13827,13 +15209,14 @@
       <c r="J104" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="G3:M3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G1:M1"/>
     <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13844,8 +15227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:B40"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13854,7 +15237,7 @@
     <col min="2" max="2" width="17.109375" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.109375" style="19"/>
     <col min="9" max="9" width="9.109375" style="19" customWidth="1"/>
@@ -13870,32 +15253,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="44"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
       <c r="N1" s="17"/>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
       <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -13972,27 +15355,27 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
       <c r="N3" s="17"/>
       <c r="P3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="Q3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
       <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -14062,10 +15445,10 @@
         <v>285.48</v>
       </c>
       <c r="C5"/>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="43"/>
+      <c r="E5" s="44"/>
       <c r="F5" s="6">
         <v>2</v>
       </c>
@@ -14481,10 +15864,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="43"/>
+      <c r="B12" s="44"/>
       <c r="D12" s="6">
         <v>2048</v>
       </c>
@@ -14720,10 +16103,10 @@
         <v>1051.98</v>
       </c>
       <c r="C16"/>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="6">
         <v>13</v>
       </c>
@@ -15074,10 +16457,10 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="47"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="39"/>
       <c r="D22" s="6">
         <v>16</v>
@@ -15199,7 +16582,7 @@
         <f>A3/B24</f>
         <v>8</v>
       </c>
-      <c r="B24" s="48">
+      <c r="B24" s="49">
         <v>8</v>
       </c>
       <c r="D24" s="10"/>
@@ -15256,7 +16639,7 @@
         <f>A4/B24</f>
         <v>16</v>
       </c>
-      <c r="B25" s="49"/>
+      <c r="B25" s="50"/>
       <c r="E25" s="1"/>
       <c r="F25" s="6">
         <v>22</v>
@@ -15310,7 +16693,7 @@
         <f>A5/B24</f>
         <v>32</v>
       </c>
-      <c r="B26" s="49"/>
+      <c r="B26" s="50"/>
       <c r="E26" s="1"/>
       <c r="F26" s="6">
         <v>23</v>
@@ -15364,7 +16747,7 @@
         <f>A6/B24</f>
         <v>64</v>
       </c>
-      <c r="B27" s="49"/>
+      <c r="B27" s="50"/>
       <c r="E27" s="1"/>
       <c r="F27" s="6">
         <v>24</v>
@@ -15418,7 +16801,7 @@
         <f>A7/B24</f>
         <v>128</v>
       </c>
-      <c r="B28" s="49"/>
+      <c r="B28" s="50"/>
       <c r="E28" s="1"/>
       <c r="F28" s="6">
         <v>25</v>
@@ -15472,7 +16855,7 @@
         <f>A8/B24</f>
         <v>256</v>
       </c>
-      <c r="B29" s="49"/>
+      <c r="B29" s="50"/>
       <c r="E29" s="1"/>
       <c r="F29" s="6">
         <v>26</v>
@@ -15526,7 +16909,7 @@
         <f>A9/B24</f>
         <v>512</v>
       </c>
-      <c r="B30" s="49"/>
+      <c r="B30" s="50"/>
       <c r="F30" s="6">
         <v>27</v>
       </c>
@@ -15624,11 +17007,11 @@
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
       <c r="E32" s="1"/>
       <c r="F32" s="6">
         <v>29</v>
@@ -16199,10 +17582,14 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="46"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="47"/>
       <c r="F42" s="6">
         <v>39</v>
       </c>
@@ -16253,7 +17640,13 @@
       <c r="B43" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="43" t="s">
         <v>27</v>
       </c>
       <c r="F43" s="6">
@@ -16307,9 +17700,17 @@
         <f>('Seq. Results'!B3+'Seq. Results'!E13)/(B3-E7) - B34</f>
         <v>1.7444756998069771E-2</v>
       </c>
-      <c r="C44" s="42">
+      <c r="C44" s="52">
         <f>B34-('Seq. Results'!B3-'Seq. Results'!E13)/(B3+E7)</f>
         <v>1.6003102759232612E-2</v>
+      </c>
+      <c r="D44" s="16">
+        <f>((B34+B44)/A24) - C34</f>
+        <v>2.1805946247587214E-3</v>
+      </c>
+      <c r="E44" s="42">
+        <f>C34-((B34-C44)/A24)</f>
+        <v>2.0003878449040766E-3</v>
       </c>
       <c r="F44" s="6">
         <v>41</v>
@@ -16362,9 +17763,17 @@
         <f>('Seq. Results'!B4+'Seq. Results'!E14)/(B4-E8) - B35</f>
         <v>2.9219082494406301E-2</v>
       </c>
-      <c r="C45" s="42">
+      <c r="C45" s="52">
         <f>B35-('Seq. Results'!B4-'Seq. Results'!E14)/(B4+E8)</f>
         <v>2.7451846608023744E-2</v>
+      </c>
+      <c r="D45" s="16">
+        <f t="shared" ref="D45:D50" si="1">((B35+B45)/A25) - C35</f>
+        <v>1.8261926559003938E-3</v>
+      </c>
+      <c r="E45" s="42">
+        <f t="shared" ref="E45:E50" si="2">C35-((B35-C45)/A25)</f>
+        <v>1.715740413001484E-3</v>
       </c>
       <c r="F45" s="6">
         <v>42</v>
@@ -16417,9 +17826,17 @@
         <f>('Seq. Results'!B5+'Seq. Results'!E15)/(B5-E9) - B36</f>
         <v>2.9908795413046141E-2</v>
       </c>
-      <c r="C46" s="42">
+      <c r="C46" s="52">
         <f>B36-('Seq. Results'!B5-'Seq. Results'!E15)/(B5+E9)</f>
         <v>2.9045166356023167E-2</v>
+      </c>
+      <c r="D46" s="16">
+        <f t="shared" si="1"/>
+        <v>9.346498566576919E-4</v>
+      </c>
+      <c r="E46" s="42">
+        <f t="shared" si="2"/>
+        <v>9.0766144862572395E-4</v>
       </c>
       <c r="F46" s="6">
         <v>43</v>
@@ -16472,9 +17889,17 @@
         <f>('Seq. Results'!B6+'Seq. Results'!E16)/(B6-E10) - B37</f>
         <v>3.870168981476052E-2</v>
       </c>
-      <c r="C47" s="42">
+      <c r="C47" s="52">
         <f>B37-('Seq. Results'!B6-'Seq. Results'!E16)/(B6+E10)</f>
         <v>3.7978282803384555E-2</v>
+      </c>
+      <c r="D47" s="16">
+        <f t="shared" si="1"/>
+        <v>6.0471390335563313E-4</v>
+      </c>
+      <c r="E47" s="42">
+        <f t="shared" si="2"/>
+        <v>5.9341066880288368E-4</v>
       </c>
       <c r="F47" s="6">
         <v>44</v>
@@ -16527,9 +17952,17 @@
         <f>('Seq. Results'!B7+'Seq. Results'!E17)/(B7-E11) - B38</f>
         <v>3.855226750576346E-2</v>
       </c>
-      <c r="C48" s="42">
+      <c r="C48" s="52">
         <f>B38-('Seq. Results'!B7-'Seq. Results'!E17)/(B7+E11)</f>
         <v>3.8208409174706581E-2</v>
+      </c>
+      <c r="D48" s="16">
+        <f t="shared" si="1"/>
+        <v>3.0118958988877703E-4</v>
+      </c>
+      <c r="E48" s="42">
+        <f t="shared" si="2"/>
+        <v>2.9850319667739517E-4</v>
       </c>
       <c r="F48" s="6">
         <v>45</v>
@@ -16582,9 +18015,17 @@
         <f>('Seq. Results'!B8+'Seq. Results'!E18)/(B8-E12) - B39</f>
         <v>5.5918063938335649E-2</v>
       </c>
-      <c r="C49" s="42">
+      <c r="C49" s="52">
         <f>B39-('Seq. Results'!B8-'Seq. Results'!E18)/(B8+E12)</f>
         <v>5.5331335328913767E-2</v>
+      </c>
+      <c r="D49" s="16">
+        <f t="shared" si="1"/>
+        <v>2.1842993725912363E-4</v>
+      </c>
+      <c r="E49" s="42">
+        <f t="shared" si="2"/>
+        <v>2.161380286285694E-4</v>
       </c>
       <c r="F49" s="6">
         <v>46</v>
@@ -16637,9 +18078,17 @@
         <f>('Seq. Results'!B9+'Seq. Results'!E19)/(B9-E13) - B40</f>
         <v>6.1641128484716035E-2</v>
       </c>
-      <c r="C50" s="42">
+      <c r="C50" s="52">
         <f>B40-('Seq. Results'!B9-'Seq. Results'!E19)/(B9+E13)</f>
         <v>6.1166544585375959E-2</v>
+      </c>
+      <c r="D50" s="16">
+        <f t="shared" si="1"/>
+        <v>1.2039282907171101E-4</v>
+      </c>
+      <c r="E50" s="42">
+        <f t="shared" si="2"/>
+        <v>1.1946590739331242E-4</v>
       </c>
       <c r="F50" s="6">
         <v>47</v>
@@ -19179,7 +20628,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="Q1:V1"/>
     <mergeCell ref="G3:M3"/>
     <mergeCell ref="Q3:V3"/>
@@ -19192,6 +20641,7 @@
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D42:E42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19217,12 +20667,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
@@ -19477,10 +20927,10 @@
       <c r="BB7" s="1"/>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="44"/>
       <c r="H8">
         <v>1268</v>
       </c>

</xml_diff>

<commit_message>
Final commit before proof-reading.
</commit_message>
<xml_diff>
--- a/Coursework Part 2/results.xlsx
+++ b/Coursework Part 2/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Seq. Results" sheetId="1" r:id="rId1"/>
@@ -846,6 +846,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,6 +861,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -866,12 +872,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -7886,7 +7886,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0"/>
+    <sheetView zoomScale="97" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -8406,32 +8406,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="45"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
       <c r="N1" s="17"/>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
       <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -8508,27 +8508,27 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
       <c r="N3" s="17"/>
       <c r="P3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="45" t="s">
+      <c r="Q3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
       <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -8936,10 +8936,10 @@
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -8988,10 +8988,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="44"/>
+      <c r="B12" s="45"/>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
@@ -11856,23 +11856,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="45"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
       <c r="Q1" s="19"/>
       <c r="R1" s="19"/>
       <c r="S1" s="19"/>
@@ -11940,15 +11940,15 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
       <c r="O3" s="10"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="19"/>
@@ -12272,10 +12272,10 @@
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="6">
         <v>8</v>
       </c>
@@ -12752,11 +12752,11 @@
       <c r="V21" s="19"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
       <c r="D22"/>
       <c r="E22" s="1"/>
       <c r="F22" s="6">
@@ -13163,14 +13163,14 @@
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="47" t="s">
+      <c r="C33" s="45"/>
+      <c r="D33" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="47"/>
+      <c r="E33" s="48"/>
       <c r="F33" s="6">
         <v>30</v>
       </c>
@@ -15227,8 +15227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:E50"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15253,32 +15253,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="45"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
       <c r="N1" s="17"/>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
       <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -15355,27 +15355,27 @@
       <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
       <c r="N3" s="17"/>
       <c r="P3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="45" t="s">
+      <c r="Q3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
       <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -15445,10 +15445,10 @@
         <v>285.48</v>
       </c>
       <c r="C5"/>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="45"/>
       <c r="F5" s="6">
         <v>2</v>
       </c>
@@ -15864,10 +15864,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="44"/>
+      <c r="B12" s="45"/>
       <c r="D12" s="6">
         <v>2048</v>
       </c>
@@ -16103,10 +16103,10 @@
         <v>1051.98</v>
       </c>
       <c r="C16"/>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="44"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="6">
         <v>13</v>
       </c>
@@ -16457,10 +16457,10 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="48"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="39"/>
       <c r="D22" s="6">
         <v>16</v>
@@ -16582,7 +16582,7 @@
         <f>A3/B24</f>
         <v>8</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="51">
         <v>8</v>
       </c>
       <c r="D24" s="10"/>
@@ -16639,7 +16639,7 @@
         <f>A4/B24</f>
         <v>16</v>
       </c>
-      <c r="B25" s="50"/>
+      <c r="B25" s="52"/>
       <c r="E25" s="1"/>
       <c r="F25" s="6">
         <v>22</v>
@@ -16693,7 +16693,7 @@
         <f>A5/B24</f>
         <v>32</v>
       </c>
-      <c r="B26" s="50"/>
+      <c r="B26" s="52"/>
       <c r="E26" s="1"/>
       <c r="F26" s="6">
         <v>23</v>
@@ -16747,7 +16747,7 @@
         <f>A6/B24</f>
         <v>64</v>
       </c>
-      <c r="B27" s="50"/>
+      <c r="B27" s="52"/>
       <c r="E27" s="1"/>
       <c r="F27" s="6">
         <v>24</v>
@@ -16801,7 +16801,7 @@
         <f>A7/B24</f>
         <v>128</v>
       </c>
-      <c r="B28" s="50"/>
+      <c r="B28" s="52"/>
       <c r="E28" s="1"/>
       <c r="F28" s="6">
         <v>25</v>
@@ -16855,7 +16855,7 @@
         <f>A8/B24</f>
         <v>256</v>
       </c>
-      <c r="B29" s="50"/>
+      <c r="B29" s="52"/>
       <c r="E29" s="1"/>
       <c r="F29" s="6">
         <v>26</v>
@@ -16909,7 +16909,7 @@
         <f>A9/B24</f>
         <v>512</v>
       </c>
-      <c r="B30" s="50"/>
+      <c r="B30" s="52"/>
       <c r="F30" s="6">
         <v>27</v>
       </c>
@@ -17007,11 +17007,11 @@
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
       <c r="E32" s="1"/>
       <c r="F32" s="6">
         <v>29</v>
@@ -17582,14 +17582,14 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="47" t="s">
+      <c r="C42" s="49"/>
+      <c r="D42" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="47"/>
+      <c r="E42" s="48"/>
       <c r="F42" s="6">
         <v>39</v>
       </c>
@@ -17700,7 +17700,7 @@
         <f>('Seq. Results'!B3+'Seq. Results'!E13)/(B3-E7) - B34</f>
         <v>1.7444756998069771E-2</v>
       </c>
-      <c r="C44" s="52">
+      <c r="C44" s="44">
         <f>B34-('Seq. Results'!B3-'Seq. Results'!E13)/(B3+E7)</f>
         <v>1.6003102759232612E-2</v>
       </c>
@@ -17763,7 +17763,7 @@
         <f>('Seq. Results'!B4+'Seq. Results'!E14)/(B4-E8) - B35</f>
         <v>2.9219082494406301E-2</v>
       </c>
-      <c r="C45" s="52">
+      <c r="C45" s="44">
         <f>B35-('Seq. Results'!B4-'Seq. Results'!E14)/(B4+E8)</f>
         <v>2.7451846608023744E-2</v>
       </c>
@@ -17826,7 +17826,7 @@
         <f>('Seq. Results'!B5+'Seq. Results'!E15)/(B5-E9) - B36</f>
         <v>2.9908795413046141E-2</v>
       </c>
-      <c r="C46" s="52">
+      <c r="C46" s="44">
         <f>B36-('Seq. Results'!B5-'Seq. Results'!E15)/(B5+E9)</f>
         <v>2.9045166356023167E-2</v>
       </c>
@@ -17889,7 +17889,7 @@
         <f>('Seq. Results'!B6+'Seq. Results'!E16)/(B6-E10) - B37</f>
         <v>3.870168981476052E-2</v>
       </c>
-      <c r="C47" s="52">
+      <c r="C47" s="44">
         <f>B37-('Seq. Results'!B6-'Seq. Results'!E16)/(B6+E10)</f>
         <v>3.7978282803384555E-2</v>
       </c>
@@ -17952,7 +17952,7 @@
         <f>('Seq. Results'!B7+'Seq. Results'!E17)/(B7-E11) - B38</f>
         <v>3.855226750576346E-2</v>
       </c>
-      <c r="C48" s="52">
+      <c r="C48" s="44">
         <f>B38-('Seq. Results'!B7-'Seq. Results'!E17)/(B7+E11)</f>
         <v>3.8208409174706581E-2</v>
       </c>
@@ -18015,7 +18015,7 @@
         <f>('Seq. Results'!B8+'Seq. Results'!E18)/(B8-E12) - B39</f>
         <v>5.5918063938335649E-2</v>
       </c>
-      <c r="C49" s="52">
+      <c r="C49" s="44">
         <f>B39-('Seq. Results'!B8-'Seq. Results'!E18)/(B8+E12)</f>
         <v>5.5331335328913767E-2</v>
       </c>
@@ -18078,7 +18078,7 @@
         <f>('Seq. Results'!B9+'Seq. Results'!E19)/(B9-E13) - B40</f>
         <v>6.1641128484716035E-2</v>
       </c>
-      <c r="C50" s="52">
+      <c r="C50" s="44">
         <f>B40-('Seq. Results'!B9-'Seq. Results'!E19)/(B9+E13)</f>
         <v>6.1166544585375959E-2</v>
       </c>
@@ -20651,8 +20651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20667,12 +20667,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
@@ -20927,10 +20927,10 @@
       <c r="BB7" s="1"/>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="45"/>
       <c r="H8">
         <v>1268</v>
       </c>

</xml_diff>